<commit_message>
fix sizes to fit page
</commit_message>
<xml_diff>
--- a/calendar.xlsx
+++ b/calendar.xlsx
@@ -62,7 +62,7 @@
       <name val="A Dast Nevis"/>
       <b val="1"/>
       <color rgb="002C363F"/>
-      <sz val="48"/>
+      <sz val="35"/>
     </font>
     <font>
       <name val="A Dast Nevis"/>
@@ -80,13 +80,13 @@
       <name val="Calibri"/>
       <b val="1"/>
       <color rgb="002C363F"/>
-      <sz val="11"/>
+      <sz val="9"/>
     </font>
     <font>
       <name val="A Dast Nevis"/>
       <b val="1"/>
       <color rgb="002C363F"/>
-      <sz val="11"/>
+      <sz val="9"/>
     </font>
   </fonts>
   <fills count="5">
@@ -534,20 +534,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="11" customWidth="1" min="7" max="7"/>
-    <col width="11" customWidth="1" min="8" max="8"/>
-    <col width="11" customWidth="1" min="9" max="9"/>
-    <col width="11" customWidth="1" min="10" max="10"/>
-    <col width="11" customWidth="1" min="11" max="11"/>
-    <col width="11" customWidth="1" min="12" max="12"/>
-    <col width="11" customWidth="1" min="13" max="13"/>
-    <col width="11" customWidth="1" min="14" max="14"/>
+    <col width="8.5" customWidth="1" min="1" max="1"/>
+    <col width="8.5" customWidth="1" min="2" max="2"/>
+    <col width="8.5" customWidth="1" min="3" max="3"/>
+    <col width="8.5" customWidth="1" min="4" max="4"/>
+    <col width="8.5" customWidth="1" min="5" max="5"/>
+    <col width="8.5" customWidth="1" min="6" max="6"/>
+    <col width="8.5" customWidth="1" min="7" max="7"/>
+    <col width="8.5" customWidth="1" min="8" max="8"/>
+    <col width="8.5" customWidth="1" min="9" max="9"/>
+    <col width="8.5" customWidth="1" min="10" max="10"/>
+    <col width="8.5" customWidth="1" min="11" max="11"/>
+    <col width="8.5" customWidth="1" min="12" max="12"/>
+    <col width="8.5" customWidth="1" min="13" max="13"/>
+    <col width="8.5" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="50" customHeight="1">
@@ -634,7 +634,7 @@
       </c>
       <c r="O3" s="3" t="n"/>
     </row>
-    <row r="4" ht="35" customHeight="1">
+    <row r="4" ht="30" customHeight="1">
       <c r="A4" s="8" t="n"/>
       <c r="B4" s="9" t="n"/>
       <c r="C4" s="8" t="n"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="O4" s="3" t="n"/>
     </row>
-    <row r="5" ht="35" customHeight="1">
+    <row r="5" ht="30" customHeight="1">
       <c r="A5" s="8" t="n"/>
       <c r="B5" s="9" t="n"/>
       <c r="C5" s="8" t="n"/>
@@ -728,7 +728,7 @@
       </c>
       <c r="O5" s="3" t="n"/>
     </row>
-    <row r="6" ht="35" customHeight="1">
+    <row r="6" ht="30" customHeight="1">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>۶</t>
@@ -801,7 +801,7 @@
       </c>
       <c r="O6" s="3" t="n"/>
     </row>
-    <row r="7" ht="35" customHeight="1">
+    <row r="7" ht="30" customHeight="1">
       <c r="A7" s="8" t="n"/>
       <c r="B7" s="9" t="inlineStr">
         <is>
@@ -846,7 +846,7 @@
       </c>
       <c r="O7" s="3" t="n"/>
     </row>
-    <row r="8" ht="35" customHeight="1">
+    <row r="8" ht="30" customHeight="1">
       <c r="A8" s="8" t="inlineStr">
         <is>
           <t>۱۳</t>
@@ -919,7 +919,7 @@
       </c>
       <c r="O8" s="3" t="n"/>
     </row>
-    <row r="9" ht="35" customHeight="1">
+    <row r="9" ht="30" customHeight="1">
       <c r="A9" s="8" t="n"/>
       <c r="B9" s="9" t="inlineStr">
         <is>
@@ -964,7 +964,7 @@
       </c>
       <c r="O9" s="3" t="n"/>
     </row>
-    <row r="10" ht="35" customHeight="1">
+    <row r="10" ht="30" customHeight="1">
       <c r="A10" s="8" t="inlineStr">
         <is>
           <t>۲۰</t>
@@ -1037,7 +1037,7 @@
       </c>
       <c r="O10" s="3" t="n"/>
     </row>
-    <row r="11" ht="35" customHeight="1">
+    <row r="11" ht="30" customHeight="1">
       <c r="A11" s="8" t="n"/>
       <c r="B11" s="9" t="inlineStr">
         <is>
@@ -1082,7 +1082,7 @@
       </c>
       <c r="O11" s="3" t="n"/>
     </row>
-    <row r="12" ht="35" customHeight="1">
+    <row r="12" ht="30" customHeight="1">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>۲۷</t>
@@ -1139,7 +1139,7 @@
       <c r="N12" s="9" t="n"/>
       <c r="O12" s="3" t="n"/>
     </row>
-    <row r="13" ht="35" customHeight="1">
+    <row r="13" ht="30" customHeight="1">
       <c r="A13" s="8" t="n"/>
       <c r="B13" s="9" t="inlineStr">
         <is>
@@ -1176,7 +1176,7 @@
       <c r="N13" s="9" t="n"/>
       <c r="O13" s="3" t="n"/>
     </row>
-    <row r="14" ht="35" customHeight="1">
+    <row r="14" ht="30" customHeight="1">
       <c r="A14" s="8" t="n"/>
       <c r="B14" s="9" t="n"/>
       <c r="C14" s="8" t="n"/>
@@ -1193,7 +1193,7 @@
       <c r="N14" s="9" t="n"/>
       <c r="O14" s="3" t="n"/>
     </row>
-    <row r="15" ht="35" customHeight="1">
+    <row r="15" ht="30" customHeight="1">
       <c r="A15" s="8" t="n"/>
       <c r="B15" s="9" t="n"/>
       <c r="C15" s="8" t="n"/>
@@ -1340,6 +1340,7 @@
     <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -1357,20 +1358,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="11" customWidth="1" min="7" max="7"/>
-    <col width="11" customWidth="1" min="8" max="8"/>
-    <col width="11" customWidth="1" min="9" max="9"/>
-    <col width="11" customWidth="1" min="10" max="10"/>
-    <col width="11" customWidth="1" min="11" max="11"/>
-    <col width="11" customWidth="1" min="12" max="12"/>
-    <col width="11" customWidth="1" min="13" max="13"/>
-    <col width="11" customWidth="1" min="14" max="14"/>
+    <col width="8.5" customWidth="1" min="1" max="1"/>
+    <col width="8.5" customWidth="1" min="2" max="2"/>
+    <col width="8.5" customWidth="1" min="3" max="3"/>
+    <col width="8.5" customWidth="1" min="4" max="4"/>
+    <col width="8.5" customWidth="1" min="5" max="5"/>
+    <col width="8.5" customWidth="1" min="6" max="6"/>
+    <col width="8.5" customWidth="1" min="7" max="7"/>
+    <col width="8.5" customWidth="1" min="8" max="8"/>
+    <col width="8.5" customWidth="1" min="9" max="9"/>
+    <col width="8.5" customWidth="1" min="10" max="10"/>
+    <col width="8.5" customWidth="1" min="11" max="11"/>
+    <col width="8.5" customWidth="1" min="12" max="12"/>
+    <col width="8.5" customWidth="1" min="13" max="13"/>
+    <col width="8.5" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="50" customHeight="1">
@@ -1457,7 +1458,7 @@
       </c>
       <c r="O3" s="3" t="n"/>
     </row>
-    <row r="4" ht="35" customHeight="1">
+    <row r="4" ht="30" customHeight="1">
       <c r="A4" s="8" t="n"/>
       <c r="B4" s="9" t="n"/>
       <c r="C4" s="8" t="n"/>
@@ -1490,7 +1491,7 @@
       </c>
       <c r="O4" s="3" t="n"/>
     </row>
-    <row r="5" ht="35" customHeight="1">
+    <row r="5" ht="30" customHeight="1">
       <c r="A5" s="8" t="n"/>
       <c r="B5" s="9" t="n"/>
       <c r="C5" s="8" t="n"/>
@@ -1515,7 +1516,7 @@
       </c>
       <c r="O5" s="3" t="n"/>
     </row>
-    <row r="6" ht="35" customHeight="1">
+    <row r="6" ht="30" customHeight="1">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>۳</t>
@@ -1588,7 +1589,7 @@
       </c>
       <c r="O6" s="3" t="n"/>
     </row>
-    <row r="7" ht="35" customHeight="1">
+    <row r="7" ht="30" customHeight="1">
       <c r="A7" s="8" t="n"/>
       <c r="B7" s="9" t="inlineStr">
         <is>
@@ -1633,7 +1634,7 @@
       </c>
       <c r="O7" s="3" t="n"/>
     </row>
-    <row r="8" ht="35" customHeight="1">
+    <row r="8" ht="30" customHeight="1">
       <c r="A8" s="8" t="inlineStr">
         <is>
           <t>۱۰</t>
@@ -1706,7 +1707,7 @@
       </c>
       <c r="O8" s="3" t="n"/>
     </row>
-    <row r="9" ht="35" customHeight="1">
+    <row r="9" ht="30" customHeight="1">
       <c r="A9" s="8" t="n"/>
       <c r="B9" s="9" t="inlineStr">
         <is>
@@ -1751,7 +1752,7 @@
       </c>
       <c r="O9" s="3" t="n"/>
     </row>
-    <row r="10" ht="35" customHeight="1">
+    <row r="10" ht="30" customHeight="1">
       <c r="A10" s="8" t="inlineStr">
         <is>
           <t>۱۷</t>
@@ -1824,7 +1825,7 @@
       </c>
       <c r="O10" s="3" t="n"/>
     </row>
-    <row r="11" ht="35" customHeight="1">
+    <row r="11" ht="30" customHeight="1">
       <c r="A11" s="8" t="n"/>
       <c r="B11" s="9" t="inlineStr">
         <is>
@@ -1869,7 +1870,7 @@
       </c>
       <c r="O11" s="3" t="n"/>
     </row>
-    <row r="12" ht="35" customHeight="1">
+    <row r="12" ht="30" customHeight="1">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>۲۴</t>
@@ -1942,7 +1943,7 @@
       </c>
       <c r="O12" s="3" t="n"/>
     </row>
-    <row r="13" ht="35" customHeight="1">
+    <row r="13" ht="30" customHeight="1">
       <c r="A13" s="8" t="n"/>
       <c r="B13" s="9" t="inlineStr">
         <is>
@@ -1987,7 +1988,7 @@
       </c>
       <c r="O13" s="3" t="n"/>
     </row>
-    <row r="14" ht="35" customHeight="1">
+    <row r="14" ht="30" customHeight="1">
       <c r="A14" s="8" t="n"/>
       <c r="B14" s="9" t="n"/>
       <c r="C14" s="8" t="n"/>
@@ -2004,7 +2005,7 @@
       <c r="N14" s="9" t="n"/>
       <c r="O14" s="3" t="n"/>
     </row>
-    <row r="15" ht="35" customHeight="1">
+    <row r="15" ht="30" customHeight="1">
       <c r="A15" s="8" t="n"/>
       <c r="B15" s="9" t="n"/>
       <c r="C15" s="8" t="n"/>
@@ -2150,6 +2151,7 @@
     <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -2167,20 +2169,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="11" customWidth="1" min="7" max="7"/>
-    <col width="11" customWidth="1" min="8" max="8"/>
-    <col width="11" customWidth="1" min="9" max="9"/>
-    <col width="11" customWidth="1" min="10" max="10"/>
-    <col width="11" customWidth="1" min="11" max="11"/>
-    <col width="11" customWidth="1" min="12" max="12"/>
-    <col width="11" customWidth="1" min="13" max="13"/>
-    <col width="11" customWidth="1" min="14" max="14"/>
+    <col width="8.5" customWidth="1" min="1" max="1"/>
+    <col width="8.5" customWidth="1" min="2" max="2"/>
+    <col width="8.5" customWidth="1" min="3" max="3"/>
+    <col width="8.5" customWidth="1" min="4" max="4"/>
+    <col width="8.5" customWidth="1" min="5" max="5"/>
+    <col width="8.5" customWidth="1" min="6" max="6"/>
+    <col width="8.5" customWidth="1" min="7" max="7"/>
+    <col width="8.5" customWidth="1" min="8" max="8"/>
+    <col width="8.5" customWidth="1" min="9" max="9"/>
+    <col width="8.5" customWidth="1" min="10" max="10"/>
+    <col width="8.5" customWidth="1" min="11" max="11"/>
+    <col width="8.5" customWidth="1" min="12" max="12"/>
+    <col width="8.5" customWidth="1" min="13" max="13"/>
+    <col width="8.5" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="50" customHeight="1">
@@ -2267,7 +2269,7 @@
       </c>
       <c r="O3" s="3" t="n"/>
     </row>
-    <row r="4" ht="35" customHeight="1">
+    <row r="4" ht="30" customHeight="1">
       <c r="A4" s="8" t="inlineStr">
         <is>
           <t>۱</t>
@@ -2340,7 +2342,7 @@
       </c>
       <c r="O4" s="3" t="n"/>
     </row>
-    <row r="5" ht="35" customHeight="1">
+    <row r="5" ht="30" customHeight="1">
       <c r="A5" s="8" t="n"/>
       <c r="B5" s="9" t="inlineStr">
         <is>
@@ -2385,7 +2387,7 @@
       </c>
       <c r="O5" s="3" t="n"/>
     </row>
-    <row r="6" ht="35" customHeight="1">
+    <row r="6" ht="30" customHeight="1">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>۸</t>
@@ -2458,7 +2460,7 @@
       </c>
       <c r="O6" s="3" t="n"/>
     </row>
-    <row r="7" ht="35" customHeight="1">
+    <row r="7" ht="30" customHeight="1">
       <c r="A7" s="8" t="n"/>
       <c r="B7" s="9" t="inlineStr">
         <is>
@@ -2503,7 +2505,7 @@
       </c>
       <c r="O7" s="3" t="n"/>
     </row>
-    <row r="8" ht="35" customHeight="1">
+    <row r="8" ht="30" customHeight="1">
       <c r="A8" s="8" t="inlineStr">
         <is>
           <t>۱۵</t>
@@ -2576,7 +2578,7 @@
       </c>
       <c r="O8" s="3" t="n"/>
     </row>
-    <row r="9" ht="35" customHeight="1">
+    <row r="9" ht="30" customHeight="1">
       <c r="A9" s="8" t="n"/>
       <c r="B9" s="9" t="inlineStr">
         <is>
@@ -2621,7 +2623,7 @@
       </c>
       <c r="O9" s="3" t="n"/>
     </row>
-    <row r="10" ht="35" customHeight="1">
+    <row r="10" ht="30" customHeight="1">
       <c r="A10" s="8" t="inlineStr">
         <is>
           <t>۲۲</t>
@@ -2694,7 +2696,7 @@
       </c>
       <c r="O10" s="3" t="n"/>
     </row>
-    <row r="11" ht="35" customHeight="1">
+    <row r="11" ht="30" customHeight="1">
       <c r="A11" s="8" t="n"/>
       <c r="B11" s="9" t="inlineStr">
         <is>
@@ -2739,7 +2741,7 @@
       </c>
       <c r="O11" s="3" t="n"/>
     </row>
-    <row r="12" ht="35" customHeight="1">
+    <row r="12" ht="30" customHeight="1">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>۲۹</t>
@@ -2772,7 +2774,7 @@
       <c r="N12" s="9" t="n"/>
       <c r="O12" s="3" t="n"/>
     </row>
-    <row r="13" ht="35" customHeight="1">
+    <row r="13" ht="30" customHeight="1">
       <c r="A13" s="8" t="n"/>
       <c r="B13" s="9" t="inlineStr">
         <is>
@@ -2797,7 +2799,7 @@
       <c r="N13" s="9" t="n"/>
       <c r="O13" s="3" t="n"/>
     </row>
-    <row r="14" ht="35" customHeight="1">
+    <row r="14" ht="30" customHeight="1">
       <c r="A14" s="8" t="n"/>
       <c r="B14" s="9" t="n"/>
       <c r="C14" s="8" t="n"/>
@@ -2814,7 +2816,7 @@
       <c r="N14" s="9" t="n"/>
       <c r="O14" s="3" t="n"/>
     </row>
-    <row r="15" ht="35" customHeight="1">
+    <row r="15" ht="30" customHeight="1">
       <c r="A15" s="8" t="n"/>
       <c r="B15" s="9" t="n"/>
       <c r="C15" s="8" t="n"/>
@@ -2960,6 +2962,7 @@
     <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -2977,20 +2980,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="11" customWidth="1" min="7" max="7"/>
-    <col width="11" customWidth="1" min="8" max="8"/>
-    <col width="11" customWidth="1" min="9" max="9"/>
-    <col width="11" customWidth="1" min="10" max="10"/>
-    <col width="11" customWidth="1" min="11" max="11"/>
-    <col width="11" customWidth="1" min="12" max="12"/>
-    <col width="11" customWidth="1" min="13" max="13"/>
-    <col width="11" customWidth="1" min="14" max="14"/>
+    <col width="8.5" customWidth="1" min="1" max="1"/>
+    <col width="8.5" customWidth="1" min="2" max="2"/>
+    <col width="8.5" customWidth="1" min="3" max="3"/>
+    <col width="8.5" customWidth="1" min="4" max="4"/>
+    <col width="8.5" customWidth="1" min="5" max="5"/>
+    <col width="8.5" customWidth="1" min="6" max="6"/>
+    <col width="8.5" customWidth="1" min="7" max="7"/>
+    <col width="8.5" customWidth="1" min="8" max="8"/>
+    <col width="8.5" customWidth="1" min="9" max="9"/>
+    <col width="8.5" customWidth="1" min="10" max="10"/>
+    <col width="8.5" customWidth="1" min="11" max="11"/>
+    <col width="8.5" customWidth="1" min="12" max="12"/>
+    <col width="8.5" customWidth="1" min="13" max="13"/>
+    <col width="8.5" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="50" customHeight="1">
@@ -3077,7 +3080,7 @@
       </c>
       <c r="O3" s="3" t="n"/>
     </row>
-    <row r="4" ht="35" customHeight="1">
+    <row r="4" ht="30" customHeight="1">
       <c r="A4" s="8" t="n"/>
       <c r="B4" s="9" t="n"/>
       <c r="C4" s="8" t="n"/>
@@ -3134,7 +3137,7 @@
       </c>
       <c r="O4" s="3" t="n"/>
     </row>
-    <row r="5" ht="35" customHeight="1">
+    <row r="5" ht="30" customHeight="1">
       <c r="A5" s="8" t="n"/>
       <c r="B5" s="9" t="n"/>
       <c r="C5" s="8" t="n"/>
@@ -3171,7 +3174,7 @@
       </c>
       <c r="O5" s="3" t="n"/>
     </row>
-    <row r="6" ht="35" customHeight="1">
+    <row r="6" ht="30" customHeight="1">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>۶</t>
@@ -3244,7 +3247,7 @@
       </c>
       <c r="O6" s="3" t="n"/>
     </row>
-    <row r="7" ht="35" customHeight="1">
+    <row r="7" ht="30" customHeight="1">
       <c r="A7" s="8" t="n"/>
       <c r="B7" s="9" t="inlineStr">
         <is>
@@ -3289,7 +3292,7 @@
       </c>
       <c r="O7" s="3" t="n"/>
     </row>
-    <row r="8" ht="35" customHeight="1">
+    <row r="8" ht="30" customHeight="1">
       <c r="A8" s="8" t="inlineStr">
         <is>
           <t>۱۳</t>
@@ -3362,7 +3365,7 @@
       </c>
       <c r="O8" s="3" t="n"/>
     </row>
-    <row r="9" ht="35" customHeight="1">
+    <row r="9" ht="30" customHeight="1">
       <c r="A9" s="8" t="n"/>
       <c r="B9" s="9" t="inlineStr">
         <is>
@@ -3407,7 +3410,7 @@
       </c>
       <c r="O9" s="3" t="n"/>
     </row>
-    <row r="10" ht="35" customHeight="1">
+    <row r="10" ht="30" customHeight="1">
       <c r="A10" s="8" t="inlineStr">
         <is>
           <t>۲۰</t>
@@ -3480,7 +3483,7 @@
       </c>
       <c r="O10" s="3" t="n"/>
     </row>
-    <row r="11" ht="35" customHeight="1">
+    <row r="11" ht="30" customHeight="1">
       <c r="A11" s="8" t="n"/>
       <c r="B11" s="9" t="inlineStr">
         <is>
@@ -3525,7 +3528,7 @@
       </c>
       <c r="O11" s="3" t="n"/>
     </row>
-    <row r="12" ht="35" customHeight="1">
+    <row r="12" ht="30" customHeight="1">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>۲۷</t>
@@ -3566,7 +3569,7 @@
       <c r="N12" s="9" t="n"/>
       <c r="O12" s="3" t="n"/>
     </row>
-    <row r="13" ht="35" customHeight="1">
+    <row r="13" ht="30" customHeight="1">
       <c r="A13" s="8" t="n"/>
       <c r="B13" s="9" t="inlineStr">
         <is>
@@ -3595,7 +3598,7 @@
       <c r="N13" s="9" t="n"/>
       <c r="O13" s="3" t="n"/>
     </row>
-    <row r="14" ht="35" customHeight="1">
+    <row r="14" ht="30" customHeight="1">
       <c r="A14" s="8" t="n"/>
       <c r="B14" s="9" t="n"/>
       <c r="C14" s="8" t="n"/>
@@ -3612,7 +3615,7 @@
       <c r="N14" s="9" t="n"/>
       <c r="O14" s="3" t="n"/>
     </row>
-    <row r="15" ht="35" customHeight="1">
+    <row r="15" ht="30" customHeight="1">
       <c r="A15" s="8" t="n"/>
       <c r="B15" s="9" t="n"/>
       <c r="C15" s="8" t="n"/>
@@ -3757,6 +3760,7 @@
     <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -3774,20 +3778,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="11" customWidth="1" min="7" max="7"/>
-    <col width="11" customWidth="1" min="8" max="8"/>
-    <col width="11" customWidth="1" min="9" max="9"/>
-    <col width="11" customWidth="1" min="10" max="10"/>
-    <col width="11" customWidth="1" min="11" max="11"/>
-    <col width="11" customWidth="1" min="12" max="12"/>
-    <col width="11" customWidth="1" min="13" max="13"/>
-    <col width="11" customWidth="1" min="14" max="14"/>
+    <col width="8.5" customWidth="1" min="1" max="1"/>
+    <col width="8.5" customWidth="1" min="2" max="2"/>
+    <col width="8.5" customWidth="1" min="3" max="3"/>
+    <col width="8.5" customWidth="1" min="4" max="4"/>
+    <col width="8.5" customWidth="1" min="5" max="5"/>
+    <col width="8.5" customWidth="1" min="6" max="6"/>
+    <col width="8.5" customWidth="1" min="7" max="7"/>
+    <col width="8.5" customWidth="1" min="8" max="8"/>
+    <col width="8.5" customWidth="1" min="9" max="9"/>
+    <col width="8.5" customWidth="1" min="10" max="10"/>
+    <col width="8.5" customWidth="1" min="11" max="11"/>
+    <col width="8.5" customWidth="1" min="12" max="12"/>
+    <col width="8.5" customWidth="1" min="13" max="13"/>
+    <col width="8.5" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="50" customHeight="1">
@@ -3874,7 +3878,7 @@
       </c>
       <c r="O3" s="3" t="n"/>
     </row>
-    <row r="4" ht="35" customHeight="1">
+    <row r="4" ht="30" customHeight="1">
       <c r="A4" s="8" t="n"/>
       <c r="B4" s="9" t="n"/>
       <c r="C4" s="8" t="n"/>
@@ -3907,7 +3911,7 @@
       </c>
       <c r="O4" s="3" t="n"/>
     </row>
-    <row r="5" ht="35" customHeight="1">
+    <row r="5" ht="30" customHeight="1">
       <c r="A5" s="8" t="n"/>
       <c r="B5" s="9" t="n"/>
       <c r="C5" s="8" t="n"/>
@@ -3932,7 +3936,7 @@
       </c>
       <c r="O5" s="3" t="n"/>
     </row>
-    <row r="6" ht="35" customHeight="1">
+    <row r="6" ht="30" customHeight="1">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>۳</t>
@@ -4005,7 +4009,7 @@
       </c>
       <c r="O6" s="3" t="n"/>
     </row>
-    <row r="7" ht="35" customHeight="1">
+    <row r="7" ht="30" customHeight="1">
       <c r="A7" s="8" t="n"/>
       <c r="B7" s="9" t="inlineStr">
         <is>
@@ -4050,7 +4054,7 @@
       </c>
       <c r="O7" s="3" t="n"/>
     </row>
-    <row r="8" ht="35" customHeight="1">
+    <row r="8" ht="30" customHeight="1">
       <c r="A8" s="8" t="inlineStr">
         <is>
           <t>۱۰</t>
@@ -4123,7 +4127,7 @@
       </c>
       <c r="O8" s="3" t="n"/>
     </row>
-    <row r="9" ht="35" customHeight="1">
+    <row r="9" ht="30" customHeight="1">
       <c r="A9" s="8" t="n"/>
       <c r="B9" s="9" t="inlineStr">
         <is>
@@ -4168,7 +4172,7 @@
       </c>
       <c r="O9" s="3" t="n"/>
     </row>
-    <row r="10" ht="35" customHeight="1">
+    <row r="10" ht="30" customHeight="1">
       <c r="A10" s="8" t="inlineStr">
         <is>
           <t>۱۷</t>
@@ -4241,7 +4245,7 @@
       </c>
       <c r="O10" s="3" t="n"/>
     </row>
-    <row r="11" ht="35" customHeight="1">
+    <row r="11" ht="30" customHeight="1">
       <c r="A11" s="8" t="n"/>
       <c r="B11" s="9" t="inlineStr">
         <is>
@@ -4286,7 +4290,7 @@
       </c>
       <c r="O11" s="3" t="n"/>
     </row>
-    <row r="12" ht="35" customHeight="1">
+    <row r="12" ht="30" customHeight="1">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>۲۴</t>
@@ -4359,7 +4363,7 @@
       </c>
       <c r="O12" s="3" t="n"/>
     </row>
-    <row r="13" ht="35" customHeight="1">
+    <row r="13" ht="30" customHeight="1">
       <c r="A13" s="8" t="n"/>
       <c r="B13" s="9" t="inlineStr">
         <is>
@@ -4404,7 +4408,7 @@
       </c>
       <c r="O13" s="3" t="n"/>
     </row>
-    <row r="14" ht="35" customHeight="1">
+    <row r="14" ht="30" customHeight="1">
       <c r="A14" s="8" t="inlineStr">
         <is>
           <t>۳۱</t>
@@ -4429,7 +4433,7 @@
       <c r="N14" s="9" t="n"/>
       <c r="O14" s="3" t="n"/>
     </row>
-    <row r="15" ht="35" customHeight="1">
+    <row r="15" ht="30" customHeight="1">
       <c r="A15" s="8" t="n"/>
       <c r="B15" s="9" t="inlineStr">
         <is>
@@ -4580,6 +4584,7 @@
     <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -4597,20 +4602,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="11" customWidth="1" min="7" max="7"/>
-    <col width="11" customWidth="1" min="8" max="8"/>
-    <col width="11" customWidth="1" min="9" max="9"/>
-    <col width="11" customWidth="1" min="10" max="10"/>
-    <col width="11" customWidth="1" min="11" max="11"/>
-    <col width="11" customWidth="1" min="12" max="12"/>
-    <col width="11" customWidth="1" min="13" max="13"/>
-    <col width="11" customWidth="1" min="14" max="14"/>
+    <col width="8.5" customWidth="1" min="1" max="1"/>
+    <col width="8.5" customWidth="1" min="2" max="2"/>
+    <col width="8.5" customWidth="1" min="3" max="3"/>
+    <col width="8.5" customWidth="1" min="4" max="4"/>
+    <col width="8.5" customWidth="1" min="5" max="5"/>
+    <col width="8.5" customWidth="1" min="6" max="6"/>
+    <col width="8.5" customWidth="1" min="7" max="7"/>
+    <col width="8.5" customWidth="1" min="8" max="8"/>
+    <col width="8.5" customWidth="1" min="9" max="9"/>
+    <col width="8.5" customWidth="1" min="10" max="10"/>
+    <col width="8.5" customWidth="1" min="11" max="11"/>
+    <col width="8.5" customWidth="1" min="12" max="12"/>
+    <col width="8.5" customWidth="1" min="13" max="13"/>
+    <col width="8.5" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="50" customHeight="1">
@@ -4697,7 +4702,7 @@
       </c>
       <c r="O3" s="3" t="n"/>
     </row>
-    <row r="4" ht="35" customHeight="1">
+    <row r="4" ht="30" customHeight="1">
       <c r="A4" s="8" t="n"/>
       <c r="B4" s="9" t="n"/>
       <c r="C4" s="8" t="inlineStr">
@@ -4762,7 +4767,7 @@
       </c>
       <c r="O4" s="3" t="n"/>
     </row>
-    <row r="5" ht="35" customHeight="1">
+    <row r="5" ht="30" customHeight="1">
       <c r="A5" s="8" t="n"/>
       <c r="B5" s="9" t="n"/>
       <c r="C5" s="8" t="n"/>
@@ -4803,7 +4808,7 @@
       </c>
       <c r="O5" s="3" t="n"/>
     </row>
-    <row r="6" ht="35" customHeight="1">
+    <row r="6" ht="30" customHeight="1">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>۷</t>
@@ -4876,7 +4881,7 @@
       </c>
       <c r="O6" s="3" t="n"/>
     </row>
-    <row r="7" ht="35" customHeight="1">
+    <row r="7" ht="30" customHeight="1">
       <c r="A7" s="8" t="n"/>
       <c r="B7" s="9" t="inlineStr">
         <is>
@@ -4921,7 +4926,7 @@
       </c>
       <c r="O7" s="3" t="n"/>
     </row>
-    <row r="8" ht="35" customHeight="1">
+    <row r="8" ht="30" customHeight="1">
       <c r="A8" s="8" t="inlineStr">
         <is>
           <t>۱۴</t>
@@ -4994,7 +4999,7 @@
       </c>
       <c r="O8" s="3" t="n"/>
     </row>
-    <row r="9" ht="35" customHeight="1">
+    <row r="9" ht="30" customHeight="1">
       <c r="A9" s="8" t="n"/>
       <c r="B9" s="9" t="inlineStr">
         <is>
@@ -5039,7 +5044,7 @@
       </c>
       <c r="O9" s="3" t="n"/>
     </row>
-    <row r="10" ht="35" customHeight="1">
+    <row r="10" ht="30" customHeight="1">
       <c r="A10" s="8" t="inlineStr">
         <is>
           <t>۲۱</t>
@@ -5112,7 +5117,7 @@
       </c>
       <c r="O10" s="3" t="n"/>
     </row>
-    <row r="11" ht="35" customHeight="1">
+    <row r="11" ht="30" customHeight="1">
       <c r="A11" s="8" t="n"/>
       <c r="B11" s="9" t="inlineStr">
         <is>
@@ -5157,7 +5162,7 @@
       </c>
       <c r="O11" s="3" t="n"/>
     </row>
-    <row r="12" ht="35" customHeight="1">
+    <row r="12" ht="30" customHeight="1">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>۲۸</t>
@@ -5206,7 +5211,7 @@
       <c r="N12" s="9" t="n"/>
       <c r="O12" s="3" t="n"/>
     </row>
-    <row r="13" ht="35" customHeight="1">
+    <row r="13" ht="30" customHeight="1">
       <c r="A13" s="8" t="n"/>
       <c r="B13" s="9" t="inlineStr">
         <is>
@@ -5239,7 +5244,7 @@
       <c r="N13" s="9" t="n"/>
       <c r="O13" s="3" t="n"/>
     </row>
-    <row r="14" ht="35" customHeight="1">
+    <row r="14" ht="30" customHeight="1">
       <c r="A14" s="8" t="n"/>
       <c r="B14" s="9" t="n"/>
       <c r="C14" s="8" t="n"/>
@@ -5256,7 +5261,7 @@
       <c r="N14" s="9" t="n"/>
       <c r="O14" s="3" t="n"/>
     </row>
-    <row r="15" ht="35" customHeight="1">
+    <row r="15" ht="30" customHeight="1">
       <c r="A15" s="8" t="n"/>
       <c r="B15" s="9" t="n"/>
       <c r="C15" s="8" t="n"/>
@@ -5403,6 +5408,7 @@
     <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -5420,20 +5426,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="11" customWidth="1" min="7" max="7"/>
-    <col width="11" customWidth="1" min="8" max="8"/>
-    <col width="11" customWidth="1" min="9" max="9"/>
-    <col width="11" customWidth="1" min="10" max="10"/>
-    <col width="11" customWidth="1" min="11" max="11"/>
-    <col width="11" customWidth="1" min="12" max="12"/>
-    <col width="11" customWidth="1" min="13" max="13"/>
-    <col width="11" customWidth="1" min="14" max="14"/>
+    <col width="8.5" customWidth="1" min="1" max="1"/>
+    <col width="8.5" customWidth="1" min="2" max="2"/>
+    <col width="8.5" customWidth="1" min="3" max="3"/>
+    <col width="8.5" customWidth="1" min="4" max="4"/>
+    <col width="8.5" customWidth="1" min="5" max="5"/>
+    <col width="8.5" customWidth="1" min="6" max="6"/>
+    <col width="8.5" customWidth="1" min="7" max="7"/>
+    <col width="8.5" customWidth="1" min="8" max="8"/>
+    <col width="8.5" customWidth="1" min="9" max="9"/>
+    <col width="8.5" customWidth="1" min="10" max="10"/>
+    <col width="8.5" customWidth="1" min="11" max="11"/>
+    <col width="8.5" customWidth="1" min="12" max="12"/>
+    <col width="8.5" customWidth="1" min="13" max="13"/>
+    <col width="8.5" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="50" customHeight="1">
@@ -5520,7 +5526,7 @@
       </c>
       <c r="O3" s="3" t="n"/>
     </row>
-    <row r="4" ht="35" customHeight="1">
+    <row r="4" ht="30" customHeight="1">
       <c r="A4" s="8" t="n"/>
       <c r="B4" s="9" t="n"/>
       <c r="C4" s="8" t="n"/>
@@ -5561,7 +5567,7 @@
       </c>
       <c r="O4" s="3" t="n"/>
     </row>
-    <row r="5" ht="35" customHeight="1">
+    <row r="5" ht="30" customHeight="1">
       <c r="A5" s="8" t="n"/>
       <c r="B5" s="9" t="n"/>
       <c r="C5" s="8" t="n"/>
@@ -5590,7 +5596,7 @@
       </c>
       <c r="O5" s="3" t="n"/>
     </row>
-    <row r="6" ht="35" customHeight="1">
+    <row r="6" ht="30" customHeight="1">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>۴</t>
@@ -5663,7 +5669,7 @@
       </c>
       <c r="O6" s="3" t="n"/>
     </row>
-    <row r="7" ht="35" customHeight="1">
+    <row r="7" ht="30" customHeight="1">
       <c r="A7" s="8" t="n"/>
       <c r="B7" s="9" t="inlineStr">
         <is>
@@ -5708,7 +5714,7 @@
       </c>
       <c r="O7" s="3" t="n"/>
     </row>
-    <row r="8" ht="35" customHeight="1">
+    <row r="8" ht="30" customHeight="1">
       <c r="A8" s="8" t="inlineStr">
         <is>
           <t>۱۱</t>
@@ -5781,7 +5787,7 @@
       </c>
       <c r="O8" s="3" t="n"/>
     </row>
-    <row r="9" ht="35" customHeight="1">
+    <row r="9" ht="30" customHeight="1">
       <c r="A9" s="8" t="n"/>
       <c r="B9" s="9" t="inlineStr">
         <is>
@@ -5826,7 +5832,7 @@
       </c>
       <c r="O9" s="3" t="n"/>
     </row>
-    <row r="10" ht="35" customHeight="1">
+    <row r="10" ht="30" customHeight="1">
       <c r="A10" s="8" t="inlineStr">
         <is>
           <t>۱۸</t>
@@ -5899,7 +5905,7 @@
       </c>
       <c r="O10" s="3" t="n"/>
     </row>
-    <row r="11" ht="35" customHeight="1">
+    <row r="11" ht="30" customHeight="1">
       <c r="A11" s="8" t="n"/>
       <c r="B11" s="9" t="inlineStr">
         <is>
@@ -5944,7 +5950,7 @@
       </c>
       <c r="O11" s="3" t="n"/>
     </row>
-    <row r="12" ht="35" customHeight="1">
+    <row r="12" ht="30" customHeight="1">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>۲۵</t>
@@ -6017,7 +6023,7 @@
       </c>
       <c r="O12" s="3" t="n"/>
     </row>
-    <row r="13" ht="35" customHeight="1">
+    <row r="13" ht="30" customHeight="1">
       <c r="A13" s="8" t="n"/>
       <c r="B13" s="9" t="inlineStr">
         <is>
@@ -6062,7 +6068,7 @@
       </c>
       <c r="O13" s="3" t="n"/>
     </row>
-    <row r="14" ht="35" customHeight="1">
+    <row r="14" ht="30" customHeight="1">
       <c r="A14" s="8" t="n"/>
       <c r="B14" s="9" t="n"/>
       <c r="C14" s="8" t="n"/>
@@ -6079,7 +6085,7 @@
       <c r="N14" s="9" t="n"/>
       <c r="O14" s="3" t="n"/>
     </row>
-    <row r="15" ht="35" customHeight="1">
+    <row r="15" ht="30" customHeight="1">
       <c r="A15" s="8" t="n"/>
       <c r="B15" s="9" t="n"/>
       <c r="C15" s="8" t="n"/>
@@ -6226,6 +6232,7 @@
     <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -6243,20 +6250,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="11" customWidth="1" min="7" max="7"/>
-    <col width="11" customWidth="1" min="8" max="8"/>
-    <col width="11" customWidth="1" min="9" max="9"/>
-    <col width="11" customWidth="1" min="10" max="10"/>
-    <col width="11" customWidth="1" min="11" max="11"/>
-    <col width="11" customWidth="1" min="12" max="12"/>
-    <col width="11" customWidth="1" min="13" max="13"/>
-    <col width="11" customWidth="1" min="14" max="14"/>
+    <col width="8.5" customWidth="1" min="1" max="1"/>
+    <col width="8.5" customWidth="1" min="2" max="2"/>
+    <col width="8.5" customWidth="1" min="3" max="3"/>
+    <col width="8.5" customWidth="1" min="4" max="4"/>
+    <col width="8.5" customWidth="1" min="5" max="5"/>
+    <col width="8.5" customWidth="1" min="6" max="6"/>
+    <col width="8.5" customWidth="1" min="7" max="7"/>
+    <col width="8.5" customWidth="1" min="8" max="8"/>
+    <col width="8.5" customWidth="1" min="9" max="9"/>
+    <col width="8.5" customWidth="1" min="10" max="10"/>
+    <col width="8.5" customWidth="1" min="11" max="11"/>
+    <col width="8.5" customWidth="1" min="12" max="12"/>
+    <col width="8.5" customWidth="1" min="13" max="13"/>
+    <col width="8.5" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="50" customHeight="1">
@@ -6343,7 +6350,7 @@
       </c>
       <c r="O3" s="3" t="n"/>
     </row>
-    <row r="4" ht="35" customHeight="1">
+    <row r="4" ht="30" customHeight="1">
       <c r="A4" s="8" t="inlineStr">
         <is>
           <t>۱</t>
@@ -6416,7 +6423,7 @@
       </c>
       <c r="O4" s="3" t="n"/>
     </row>
-    <row r="5" ht="35" customHeight="1">
+    <row r="5" ht="30" customHeight="1">
       <c r="A5" s="8" t="n"/>
       <c r="B5" s="9" t="inlineStr">
         <is>
@@ -6461,7 +6468,7 @@
       </c>
       <c r="O5" s="3" t="n"/>
     </row>
-    <row r="6" ht="35" customHeight="1">
+    <row r="6" ht="30" customHeight="1">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>۸</t>
@@ -6534,7 +6541,7 @@
       </c>
       <c r="O6" s="3" t="n"/>
     </row>
-    <row r="7" ht="35" customHeight="1">
+    <row r="7" ht="30" customHeight="1">
       <c r="A7" s="8" t="n"/>
       <c r="B7" s="12" t="inlineStr">
         <is>
@@ -6579,7 +6586,7 @@
       </c>
       <c r="O7" s="3" t="n"/>
     </row>
-    <row r="8" ht="35" customHeight="1">
+    <row r="8" ht="30" customHeight="1">
       <c r="A8" s="8" t="inlineStr">
         <is>
           <t>۱۵</t>
@@ -6652,7 +6659,7 @@
       </c>
       <c r="O8" s="3" t="n"/>
     </row>
-    <row r="9" ht="35" customHeight="1">
+    <row r="9" ht="30" customHeight="1">
       <c r="A9" s="8" t="n"/>
       <c r="B9" s="9" t="inlineStr">
         <is>
@@ -6697,7 +6704,7 @@
       </c>
       <c r="O9" s="3" t="n"/>
     </row>
-    <row r="10" ht="35" customHeight="1">
+    <row r="10" ht="30" customHeight="1">
       <c r="A10" s="8" t="inlineStr">
         <is>
           <t>۲۲</t>
@@ -6770,7 +6777,7 @@
       </c>
       <c r="O10" s="3" t="n"/>
     </row>
-    <row r="11" ht="35" customHeight="1">
+    <row r="11" ht="30" customHeight="1">
       <c r="A11" s="8" t="n"/>
       <c r="B11" s="9" t="inlineStr">
         <is>
@@ -6815,7 +6822,7 @@
       </c>
       <c r="O11" s="3" t="n"/>
     </row>
-    <row r="12" ht="35" customHeight="1">
+    <row r="12" ht="30" customHeight="1">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>۲۹</t>
@@ -6856,7 +6863,7 @@
       <c r="N12" s="9" t="n"/>
       <c r="O12" s="3" t="n"/>
     </row>
-    <row r="13" ht="35" customHeight="1">
+    <row r="13" ht="30" customHeight="1">
       <c r="A13" s="8" t="n"/>
       <c r="B13" s="9" t="inlineStr">
         <is>
@@ -6885,7 +6892,7 @@
       <c r="N13" s="9" t="n"/>
       <c r="O13" s="3" t="n"/>
     </row>
-    <row r="14" ht="35" customHeight="1">
+    <row r="14" ht="30" customHeight="1">
       <c r="A14" s="8" t="n"/>
       <c r="B14" s="9" t="n"/>
       <c r="C14" s="8" t="n"/>
@@ -6902,7 +6909,7 @@
       <c r="N14" s="9" t="n"/>
       <c r="O14" s="3" t="n"/>
     </row>
-    <row r="15" ht="35" customHeight="1">
+    <row r="15" ht="30" customHeight="1">
       <c r="A15" s="8" t="n"/>
       <c r="B15" s="9" t="n"/>
       <c r="C15" s="8" t="n"/>
@@ -7049,6 +7056,7 @@
     <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -7066,20 +7074,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="11" customWidth="1" min="7" max="7"/>
-    <col width="11" customWidth="1" min="8" max="8"/>
-    <col width="11" customWidth="1" min="9" max="9"/>
-    <col width="11" customWidth="1" min="10" max="10"/>
-    <col width="11" customWidth="1" min="11" max="11"/>
-    <col width="11" customWidth="1" min="12" max="12"/>
-    <col width="11" customWidth="1" min="13" max="13"/>
-    <col width="11" customWidth="1" min="14" max="14"/>
+    <col width="8.5" customWidth="1" min="1" max="1"/>
+    <col width="8.5" customWidth="1" min="2" max="2"/>
+    <col width="8.5" customWidth="1" min="3" max="3"/>
+    <col width="8.5" customWidth="1" min="4" max="4"/>
+    <col width="8.5" customWidth="1" min="5" max="5"/>
+    <col width="8.5" customWidth="1" min="6" max="6"/>
+    <col width="8.5" customWidth="1" min="7" max="7"/>
+    <col width="8.5" customWidth="1" min="8" max="8"/>
+    <col width="8.5" customWidth="1" min="9" max="9"/>
+    <col width="8.5" customWidth="1" min="10" max="10"/>
+    <col width="8.5" customWidth="1" min="11" max="11"/>
+    <col width="8.5" customWidth="1" min="12" max="12"/>
+    <col width="8.5" customWidth="1" min="13" max="13"/>
+    <col width="8.5" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="50" customHeight="1">
@@ -7166,7 +7174,7 @@
       </c>
       <c r="O3" s="3" t="n"/>
     </row>
-    <row r="4" ht="35" customHeight="1">
+    <row r="4" ht="30" customHeight="1">
       <c r="A4" s="8" t="n"/>
       <c r="B4" s="9" t="n"/>
       <c r="C4" s="8" t="n"/>
@@ -7215,7 +7223,7 @@
       </c>
       <c r="O4" s="3" t="n"/>
     </row>
-    <row r="5" ht="35" customHeight="1">
+    <row r="5" ht="30" customHeight="1">
       <c r="A5" s="8" t="n"/>
       <c r="B5" s="9" t="n"/>
       <c r="C5" s="8" t="n"/>
@@ -7248,7 +7256,7 @@
       </c>
       <c r="O5" s="3" t="n"/>
     </row>
-    <row r="6" ht="35" customHeight="1">
+    <row r="6" ht="30" customHeight="1">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>۵</t>
@@ -7321,7 +7329,7 @@
       </c>
       <c r="O6" s="3" t="n"/>
     </row>
-    <row r="7" ht="35" customHeight="1">
+    <row r="7" ht="30" customHeight="1">
       <c r="A7" s="8" t="n"/>
       <c r="B7" s="9" t="inlineStr">
         <is>
@@ -7366,7 +7374,7 @@
       </c>
       <c r="O7" s="3" t="n"/>
     </row>
-    <row r="8" ht="35" customHeight="1">
+    <row r="8" ht="30" customHeight="1">
       <c r="A8" s="8" t="inlineStr">
         <is>
           <t>۱۲</t>
@@ -7439,7 +7447,7 @@
       </c>
       <c r="O8" s="3" t="n"/>
     </row>
-    <row r="9" ht="35" customHeight="1">
+    <row r="9" ht="30" customHeight="1">
       <c r="A9" s="8" t="n"/>
       <c r="B9" s="9" t="inlineStr">
         <is>
@@ -7484,7 +7492,7 @@
       </c>
       <c r="O9" s="3" t="n"/>
     </row>
-    <row r="10" ht="35" customHeight="1">
+    <row r="10" ht="30" customHeight="1">
       <c r="A10" s="8" t="inlineStr">
         <is>
           <t>۱۹</t>
@@ -7557,7 +7565,7 @@
       </c>
       <c r="O10" s="3" t="n"/>
     </row>
-    <row r="11" ht="35" customHeight="1">
+    <row r="11" ht="30" customHeight="1">
       <c r="A11" s="8" t="n"/>
       <c r="B11" s="9" t="inlineStr">
         <is>
@@ -7602,7 +7610,7 @@
       </c>
       <c r="O11" s="3" t="n"/>
     </row>
-    <row r="12" ht="35" customHeight="1">
+    <row r="12" ht="30" customHeight="1">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>۲۶</t>
@@ -7667,7 +7675,7 @@
       <c r="N12" s="9" t="n"/>
       <c r="O12" s="3" t="n"/>
     </row>
-    <row r="13" ht="35" customHeight="1">
+    <row r="13" ht="30" customHeight="1">
       <c r="A13" s="8" t="n"/>
       <c r="B13" s="9" t="inlineStr">
         <is>
@@ -7708,7 +7716,7 @@
       <c r="N13" s="9" t="n"/>
       <c r="O13" s="3" t="n"/>
     </row>
-    <row r="14" ht="35" customHeight="1">
+    <row r="14" ht="30" customHeight="1">
       <c r="A14" s="8" t="n"/>
       <c r="B14" s="9" t="n"/>
       <c r="C14" s="8" t="n"/>
@@ -7725,7 +7733,7 @@
       <c r="N14" s="9" t="n"/>
       <c r="O14" s="3" t="n"/>
     </row>
-    <row r="15" ht="35" customHeight="1">
+    <row r="15" ht="30" customHeight="1">
       <c r="A15" s="8" t="n"/>
       <c r="B15" s="9" t="n"/>
       <c r="C15" s="8" t="n"/>
@@ -7872,6 +7880,7 @@
     <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -7889,20 +7898,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="11" customWidth="1" min="7" max="7"/>
-    <col width="11" customWidth="1" min="8" max="8"/>
-    <col width="11" customWidth="1" min="9" max="9"/>
-    <col width="11" customWidth="1" min="10" max="10"/>
-    <col width="11" customWidth="1" min="11" max="11"/>
-    <col width="11" customWidth="1" min="12" max="12"/>
-    <col width="11" customWidth="1" min="13" max="13"/>
-    <col width="11" customWidth="1" min="14" max="14"/>
+    <col width="8.5" customWidth="1" min="1" max="1"/>
+    <col width="8.5" customWidth="1" min="2" max="2"/>
+    <col width="8.5" customWidth="1" min="3" max="3"/>
+    <col width="8.5" customWidth="1" min="4" max="4"/>
+    <col width="8.5" customWidth="1" min="5" max="5"/>
+    <col width="8.5" customWidth="1" min="6" max="6"/>
+    <col width="8.5" customWidth="1" min="7" max="7"/>
+    <col width="8.5" customWidth="1" min="8" max="8"/>
+    <col width="8.5" customWidth="1" min="9" max="9"/>
+    <col width="8.5" customWidth="1" min="10" max="10"/>
+    <col width="8.5" customWidth="1" min="11" max="11"/>
+    <col width="8.5" customWidth="1" min="12" max="12"/>
+    <col width="8.5" customWidth="1" min="13" max="13"/>
+    <col width="8.5" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="50" customHeight="1">
@@ -7989,7 +7998,7 @@
       </c>
       <c r="O3" s="3" t="n"/>
     </row>
-    <row r="4" ht="35" customHeight="1">
+    <row r="4" ht="30" customHeight="1">
       <c r="A4" s="8" t="n"/>
       <c r="B4" s="9" t="n"/>
       <c r="C4" s="8" t="n"/>
@@ -8014,7 +8023,7 @@
       </c>
       <c r="O4" s="3" t="n"/>
     </row>
-    <row r="5" ht="35" customHeight="1">
+    <row r="5" ht="30" customHeight="1">
       <c r="A5" s="8" t="n"/>
       <c r="B5" s="9" t="n"/>
       <c r="C5" s="8" t="n"/>
@@ -8035,7 +8044,7 @@
       </c>
       <c r="O5" s="3" t="n"/>
     </row>
-    <row r="6" ht="35" customHeight="1">
+    <row r="6" ht="30" customHeight="1">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>۲</t>
@@ -8108,7 +8117,7 @@
       </c>
       <c r="O6" s="3" t="n"/>
     </row>
-    <row r="7" ht="35" customHeight="1">
+    <row r="7" ht="30" customHeight="1">
       <c r="A7" s="8" t="n"/>
       <c r="B7" s="9" t="inlineStr">
         <is>
@@ -8153,7 +8162,7 @@
       </c>
       <c r="O7" s="3" t="n"/>
     </row>
-    <row r="8" ht="35" customHeight="1">
+    <row r="8" ht="30" customHeight="1">
       <c r="A8" s="8" t="inlineStr">
         <is>
           <t>۹</t>
@@ -8226,7 +8235,7 @@
       </c>
       <c r="O8" s="3" t="n"/>
     </row>
-    <row r="9" ht="35" customHeight="1">
+    <row r="9" ht="30" customHeight="1">
       <c r="A9" s="8" t="n"/>
       <c r="B9" s="9" t="inlineStr">
         <is>
@@ -8271,7 +8280,7 @@
       </c>
       <c r="O9" s="3" t="n"/>
     </row>
-    <row r="10" ht="35" customHeight="1">
+    <row r="10" ht="30" customHeight="1">
       <c r="A10" s="8" t="inlineStr">
         <is>
           <t>۱۶</t>
@@ -8344,7 +8353,7 @@
       </c>
       <c r="O10" s="3" t="n"/>
     </row>
-    <row r="11" ht="35" customHeight="1">
+    <row r="11" ht="30" customHeight="1">
       <c r="A11" s="8" t="n"/>
       <c r="B11" s="9" t="inlineStr">
         <is>
@@ -8389,7 +8398,7 @@
       </c>
       <c r="O11" s="3" t="n"/>
     </row>
-    <row r="12" ht="35" customHeight="1">
+    <row r="12" ht="30" customHeight="1">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>۲۳</t>
@@ -8462,7 +8471,7 @@
       </c>
       <c r="O12" s="3" t="n"/>
     </row>
-    <row r="13" ht="35" customHeight="1">
+    <row r="13" ht="30" customHeight="1">
       <c r="A13" s="8" t="n"/>
       <c r="B13" s="9" t="inlineStr">
         <is>
@@ -8507,7 +8516,7 @@
       </c>
       <c r="O13" s="3" t="n"/>
     </row>
-    <row r="14" ht="35" customHeight="1">
+    <row r="14" ht="30" customHeight="1">
       <c r="A14" s="8" t="inlineStr">
         <is>
           <t>۳۰</t>
@@ -8532,7 +8541,7 @@
       <c r="N14" s="9" t="n"/>
       <c r="O14" s="3" t="n"/>
     </row>
-    <row r="15" ht="35" customHeight="1">
+    <row r="15" ht="30" customHeight="1">
       <c r="A15" s="8" t="n"/>
       <c r="B15" s="9" t="inlineStr">
         <is>
@@ -8682,6 +8691,7 @@
     <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -8699,20 +8709,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="11" customWidth="1" min="7" max="7"/>
-    <col width="11" customWidth="1" min="8" max="8"/>
-    <col width="11" customWidth="1" min="9" max="9"/>
-    <col width="11" customWidth="1" min="10" max="10"/>
-    <col width="11" customWidth="1" min="11" max="11"/>
-    <col width="11" customWidth="1" min="12" max="12"/>
-    <col width="11" customWidth="1" min="13" max="13"/>
-    <col width="11" customWidth="1" min="14" max="14"/>
+    <col width="8.5" customWidth="1" min="1" max="1"/>
+    <col width="8.5" customWidth="1" min="2" max="2"/>
+    <col width="8.5" customWidth="1" min="3" max="3"/>
+    <col width="8.5" customWidth="1" min="4" max="4"/>
+    <col width="8.5" customWidth="1" min="5" max="5"/>
+    <col width="8.5" customWidth="1" min="6" max="6"/>
+    <col width="8.5" customWidth="1" min="7" max="7"/>
+    <col width="8.5" customWidth="1" min="8" max="8"/>
+    <col width="8.5" customWidth="1" min="9" max="9"/>
+    <col width="8.5" customWidth="1" min="10" max="10"/>
+    <col width="8.5" customWidth="1" min="11" max="11"/>
+    <col width="8.5" customWidth="1" min="12" max="12"/>
+    <col width="8.5" customWidth="1" min="13" max="13"/>
+    <col width="8.5" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="50" customHeight="1">
@@ -8799,7 +8809,7 @@
       </c>
       <c r="O3" s="3" t="n"/>
     </row>
-    <row r="4" ht="35" customHeight="1">
+    <row r="4" ht="30" customHeight="1">
       <c r="A4" s="8" t="n"/>
       <c r="B4" s="9" t="n"/>
       <c r="C4" s="8" t="inlineStr">
@@ -8864,7 +8874,7 @@
       </c>
       <c r="O4" s="3" t="n"/>
     </row>
-    <row r="5" ht="35" customHeight="1">
+    <row r="5" ht="30" customHeight="1">
       <c r="A5" s="8" t="n"/>
       <c r="B5" s="9" t="n"/>
       <c r="C5" s="8" t="n"/>
@@ -8905,7 +8915,7 @@
       </c>
       <c r="O5" s="3" t="n"/>
     </row>
-    <row r="6" ht="35" customHeight="1">
+    <row r="6" ht="30" customHeight="1">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>۷</t>
@@ -8978,7 +8988,7 @@
       </c>
       <c r="O6" s="3" t="n"/>
     </row>
-    <row r="7" ht="35" customHeight="1">
+    <row r="7" ht="30" customHeight="1">
       <c r="A7" s="8" t="n"/>
       <c r="B7" s="9" t="inlineStr">
         <is>
@@ -9023,7 +9033,7 @@
       </c>
       <c r="O7" s="3" t="n"/>
     </row>
-    <row r="8" ht="35" customHeight="1">
+    <row r="8" ht="30" customHeight="1">
       <c r="A8" s="8" t="inlineStr">
         <is>
           <t>۱۴</t>
@@ -9096,7 +9106,7 @@
       </c>
       <c r="O8" s="3" t="n"/>
     </row>
-    <row r="9" ht="35" customHeight="1">
+    <row r="9" ht="30" customHeight="1">
       <c r="A9" s="8" t="n"/>
       <c r="B9" s="9" t="inlineStr">
         <is>
@@ -9141,7 +9151,7 @@
       </c>
       <c r="O9" s="3" t="n"/>
     </row>
-    <row r="10" ht="35" customHeight="1">
+    <row r="10" ht="30" customHeight="1">
       <c r="A10" s="8" t="inlineStr">
         <is>
           <t>۲۱</t>
@@ -9214,7 +9224,7 @@
       </c>
       <c r="O10" s="3" t="n"/>
     </row>
-    <row r="11" ht="35" customHeight="1">
+    <row r="11" ht="30" customHeight="1">
       <c r="A11" s="8" t="n"/>
       <c r="B11" s="9" t="inlineStr">
         <is>
@@ -9259,7 +9269,7 @@
       </c>
       <c r="O11" s="3" t="n"/>
     </row>
-    <row r="12" ht="35" customHeight="1">
+    <row r="12" ht="30" customHeight="1">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>۲۸</t>
@@ -9300,7 +9310,7 @@
       <c r="N12" s="9" t="n"/>
       <c r="O12" s="3" t="n"/>
     </row>
-    <row r="13" ht="35" customHeight="1">
+    <row r="13" ht="30" customHeight="1">
       <c r="A13" s="8" t="n"/>
       <c r="B13" s="9" t="inlineStr">
         <is>
@@ -9329,7 +9339,7 @@
       <c r="N13" s="9" t="n"/>
       <c r="O13" s="3" t="n"/>
     </row>
-    <row r="14" ht="35" customHeight="1">
+    <row r="14" ht="30" customHeight="1">
       <c r="A14" s="8" t="n"/>
       <c r="B14" s="9" t="n"/>
       <c r="C14" s="8" t="n"/>
@@ -9346,7 +9356,7 @@
       <c r="N14" s="9" t="n"/>
       <c r="O14" s="3" t="n"/>
     </row>
-    <row r="15" ht="35" customHeight="1">
+    <row r="15" ht="30" customHeight="1">
       <c r="A15" s="8" t="n"/>
       <c r="B15" s="9" t="n"/>
       <c r="C15" s="8" t="n"/>
@@ -9492,6 +9502,7 @@
     <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -9509,20 +9520,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="11" customWidth="1" min="7" max="7"/>
-    <col width="11" customWidth="1" min="8" max="8"/>
-    <col width="11" customWidth="1" min="9" max="9"/>
-    <col width="11" customWidth="1" min="10" max="10"/>
-    <col width="11" customWidth="1" min="11" max="11"/>
-    <col width="11" customWidth="1" min="12" max="12"/>
-    <col width="11" customWidth="1" min="13" max="13"/>
-    <col width="11" customWidth="1" min="14" max="14"/>
+    <col width="8.5" customWidth="1" min="1" max="1"/>
+    <col width="8.5" customWidth="1" min="2" max="2"/>
+    <col width="8.5" customWidth="1" min="3" max="3"/>
+    <col width="8.5" customWidth="1" min="4" max="4"/>
+    <col width="8.5" customWidth="1" min="5" max="5"/>
+    <col width="8.5" customWidth="1" min="6" max="6"/>
+    <col width="8.5" customWidth="1" min="7" max="7"/>
+    <col width="8.5" customWidth="1" min="8" max="8"/>
+    <col width="8.5" customWidth="1" min="9" max="9"/>
+    <col width="8.5" customWidth="1" min="10" max="10"/>
+    <col width="8.5" customWidth="1" min="11" max="11"/>
+    <col width="8.5" customWidth="1" min="12" max="12"/>
+    <col width="8.5" customWidth="1" min="13" max="13"/>
+    <col width="8.5" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="50" customHeight="1">
@@ -9609,7 +9620,7 @@
       </c>
       <c r="O3" s="3" t="n"/>
     </row>
-    <row r="4" ht="35" customHeight="1">
+    <row r="4" ht="30" customHeight="1">
       <c r="A4" s="8" t="n"/>
       <c r="B4" s="9" t="n"/>
       <c r="C4" s="8" t="n"/>
@@ -9658,7 +9669,7 @@
       </c>
       <c r="O4" s="3" t="n"/>
     </row>
-    <row r="5" ht="35" customHeight="1">
+    <row r="5" ht="30" customHeight="1">
       <c r="A5" s="8" t="n"/>
       <c r="B5" s="9" t="n"/>
       <c r="C5" s="8" t="n"/>
@@ -9691,7 +9702,7 @@
       </c>
       <c r="O5" s="3" t="n"/>
     </row>
-    <row r="6" ht="35" customHeight="1">
+    <row r="6" ht="30" customHeight="1">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>۵</t>
@@ -9764,7 +9775,7 @@
       </c>
       <c r="O6" s="3" t="n"/>
     </row>
-    <row r="7" ht="35" customHeight="1">
+    <row r="7" ht="30" customHeight="1">
       <c r="A7" s="8" t="n"/>
       <c r="B7" s="9" t="inlineStr">
         <is>
@@ -9809,7 +9820,7 @@
       </c>
       <c r="O7" s="3" t="n"/>
     </row>
-    <row r="8" ht="35" customHeight="1">
+    <row r="8" ht="30" customHeight="1">
       <c r="A8" s="8" t="inlineStr">
         <is>
           <t>۱۲</t>
@@ -9882,7 +9893,7 @@
       </c>
       <c r="O8" s="3" t="n"/>
     </row>
-    <row r="9" ht="35" customHeight="1">
+    <row r="9" ht="30" customHeight="1">
       <c r="A9" s="8" t="n"/>
       <c r="B9" s="9" t="inlineStr">
         <is>
@@ -9927,7 +9938,7 @@
       </c>
       <c r="O9" s="3" t="n"/>
     </row>
-    <row r="10" ht="35" customHeight="1">
+    <row r="10" ht="30" customHeight="1">
       <c r="A10" s="8" t="inlineStr">
         <is>
           <t>۱۹</t>
@@ -10000,7 +10011,7 @@
       </c>
       <c r="O10" s="3" t="n"/>
     </row>
-    <row r="11" ht="35" customHeight="1">
+    <row r="11" ht="30" customHeight="1">
       <c r="A11" s="8" t="n"/>
       <c r="B11" s="9" t="inlineStr">
         <is>
@@ -10045,7 +10056,7 @@
       </c>
       <c r="O11" s="3" t="n"/>
     </row>
-    <row r="12" ht="35" customHeight="1">
+    <row r="12" ht="30" customHeight="1">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>۲۶</t>
@@ -10102,7 +10113,7 @@
       <c r="N12" s="9" t="n"/>
       <c r="O12" s="3" t="n"/>
     </row>
-    <row r="13" ht="35" customHeight="1">
+    <row r="13" ht="30" customHeight="1">
       <c r="A13" s="8" t="n"/>
       <c r="B13" s="9" t="inlineStr">
         <is>
@@ -10139,7 +10150,7 @@
       <c r="N13" s="9" t="n"/>
       <c r="O13" s="3" t="n"/>
     </row>
-    <row r="14" ht="35" customHeight="1">
+    <row r="14" ht="30" customHeight="1">
       <c r="A14" s="8" t="n"/>
       <c r="B14" s="9" t="n"/>
       <c r="C14" s="8" t="n"/>
@@ -10156,7 +10167,7 @@
       <c r="N14" s="9" t="n"/>
       <c r="O14" s="3" t="n"/>
     </row>
-    <row r="15" ht="35" customHeight="1">
+    <row r="15" ht="30" customHeight="1">
       <c r="A15" s="8" t="n"/>
       <c r="B15" s="9" t="n"/>
       <c r="C15" s="8" t="n"/>
@@ -10302,5 +10313,6 @@
     <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add some ui and some font name and size fixes
</commit_message>
<xml_diff>
--- a/calendar.xlsx
+++ b/calendar.xlsx
@@ -28,7 +28,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -56,35 +56,21 @@
       <name val="Far.Domrol"/>
       <b val="1"/>
       <color rgb="002C363F"/>
-      <sz val="20"/>
+      <sz val="18"/>
     </font>
     <font>
-      <name val="A Dast Nevis"/>
+      <name val="Calibri"/>
       <b val="1"/>
       <color rgb="002C363F"/>
       <sz val="35"/>
     </font>
     <font>
-      <name val="A Dast Nevis"/>
-      <b val="1"/>
+      <name val="Calibri"/>
       <color rgb="002C363F"/>
       <sz val="17"/>
     </font>
     <font>
       <name val="Calibri"/>
-      <b val="1"/>
-      <color rgb="002C363F"/>
-      <sz val="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <b val="1"/>
-      <color rgb="002C363F"/>
-      <sz val="9"/>
-    </font>
-    <font>
-      <name val="A Dast Nevis"/>
-      <b val="1"/>
       <color rgb="002C363F"/>
       <sz val="9"/>
     </font>
@@ -127,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
@@ -153,12 +139,6 @@
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
   </cellXfs>
@@ -644,7 +624,7 @@
           <t>۱</t>
         </is>
       </c>
-      <c r="F4" s="10" t="inlineStr">
+      <c r="F4" s="9" t="inlineStr">
         <is>
           <t>21</t>
         </is>
@@ -654,7 +634,7 @@
           <t>۲</t>
         </is>
       </c>
-      <c r="H4" s="10" t="inlineStr">
+      <c r="H4" s="9" t="inlineStr">
         <is>
           <t>22</t>
         </is>
@@ -664,7 +644,7 @@
           <t>۳</t>
         </is>
       </c>
-      <c r="J4" s="10" t="inlineStr">
+      <c r="J4" s="9" t="inlineStr">
         <is>
           <t>23</t>
         </is>
@@ -674,7 +654,7 @@
           <t>۴</t>
         </is>
       </c>
-      <c r="L4" s="10" t="inlineStr">
+      <c r="L4" s="9" t="inlineStr">
         <is>
           <t>24</t>
         </is>
@@ -684,7 +664,7 @@
           <t>۵</t>
         </is>
       </c>
-      <c r="N4" s="10" t="inlineStr">
+      <c r="N4" s="9" t="inlineStr">
         <is>
           <t>25</t>
         </is>
@@ -734,7 +714,7 @@
           <t>۶</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="9" t="inlineStr">
         <is>
           <t>26</t>
         </is>
@@ -744,7 +724,7 @@
           <t>۷</t>
         </is>
       </c>
-      <c r="D6" s="10" t="inlineStr">
+      <c r="D6" s="9" t="inlineStr">
         <is>
           <t>27</t>
         </is>
@@ -754,7 +734,7 @@
           <t>۸</t>
         </is>
       </c>
-      <c r="F6" s="10" t="inlineStr">
+      <c r="F6" s="9" t="inlineStr">
         <is>
           <t>28</t>
         </is>
@@ -764,7 +744,7 @@
           <t>۹</t>
         </is>
       </c>
-      <c r="H6" s="10" t="inlineStr">
+      <c r="H6" s="9" t="inlineStr">
         <is>
           <t>29</t>
         </is>
@@ -774,7 +754,7 @@
           <t>۱۰</t>
         </is>
       </c>
-      <c r="J6" s="10" t="inlineStr">
+      <c r="J6" s="9" t="inlineStr">
         <is>
           <t>30</t>
         </is>
@@ -784,7 +764,7 @@
           <t>۱۱</t>
         </is>
       </c>
-      <c r="L6" s="10" t="inlineStr">
+      <c r="L6" s="9" t="inlineStr">
         <is>
           <t>31</t>
         </is>
@@ -794,7 +774,7 @@
           <t>۱۲</t>
         </is>
       </c>
-      <c r="N6" s="11" t="inlineStr">
+      <c r="N6" s="10" t="inlineStr">
         <is>
           <t>1 April</t>
         </is>
@@ -852,7 +832,7 @@
           <t>۱۳</t>
         </is>
       </c>
-      <c r="B8" s="10" t="inlineStr">
+      <c r="B8" s="9" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -862,7 +842,7 @@
           <t>۱۴</t>
         </is>
       </c>
-      <c r="D8" s="10" t="inlineStr">
+      <c r="D8" s="9" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -872,7 +852,7 @@
           <t>۱۵</t>
         </is>
       </c>
-      <c r="F8" s="10" t="inlineStr">
+      <c r="F8" s="9" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -882,7 +862,7 @@
           <t>۱۶</t>
         </is>
       </c>
-      <c r="H8" s="10" t="inlineStr">
+      <c r="H8" s="9" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -892,7 +872,7 @@
           <t>۱۷</t>
         </is>
       </c>
-      <c r="J8" s="10" t="inlineStr">
+      <c r="J8" s="9" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -902,7 +882,7 @@
           <t>۱۸</t>
         </is>
       </c>
-      <c r="L8" s="10" t="inlineStr">
+      <c r="L8" s="9" t="inlineStr">
         <is>
           <t>7</t>
         </is>
@@ -912,7 +892,7 @@
           <t>۱۹</t>
         </is>
       </c>
-      <c r="N8" s="10" t="inlineStr">
+      <c r="N8" s="9" t="inlineStr">
         <is>
           <t>8</t>
         </is>
@@ -927,7 +907,7 @@
         </is>
       </c>
       <c r="C9" s="8" t="n"/>
-      <c r="D9" s="12" t="inlineStr">
+      <c r="D9" s="10" t="inlineStr">
         <is>
           <t>١ رمضان</t>
         </is>
@@ -970,7 +950,7 @@
           <t>۲۰</t>
         </is>
       </c>
-      <c r="B10" s="10" t="inlineStr">
+      <c r="B10" s="9" t="inlineStr">
         <is>
           <t>9</t>
         </is>
@@ -980,7 +960,7 @@
           <t>۲۱</t>
         </is>
       </c>
-      <c r="D10" s="10" t="inlineStr">
+      <c r="D10" s="9" t="inlineStr">
         <is>
           <t>10</t>
         </is>
@@ -990,7 +970,7 @@
           <t>۲۲</t>
         </is>
       </c>
-      <c r="F10" s="10" t="inlineStr">
+      <c r="F10" s="9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
@@ -1000,7 +980,7 @@
           <t>۲۳</t>
         </is>
       </c>
-      <c r="H10" s="10" t="inlineStr">
+      <c r="H10" s="9" t="inlineStr">
         <is>
           <t>12</t>
         </is>
@@ -1010,7 +990,7 @@
           <t>۲۴</t>
         </is>
       </c>
-      <c r="J10" s="10" t="inlineStr">
+      <c r="J10" s="9" t="inlineStr">
         <is>
           <t>13</t>
         </is>
@@ -1020,7 +1000,7 @@
           <t>۲۵</t>
         </is>
       </c>
-      <c r="L10" s="10" t="inlineStr">
+      <c r="L10" s="9" t="inlineStr">
         <is>
           <t>14</t>
         </is>
@@ -1030,7 +1010,7 @@
           <t>۲۶</t>
         </is>
       </c>
-      <c r="N10" s="10" t="inlineStr">
+      <c r="N10" s="9" t="inlineStr">
         <is>
           <t>15</t>
         </is>
@@ -1088,7 +1068,7 @@
           <t>۲۷</t>
         </is>
       </c>
-      <c r="B12" s="10" t="inlineStr">
+      <c r="B12" s="9" t="inlineStr">
         <is>
           <t>16</t>
         </is>
@@ -1098,7 +1078,7 @@
           <t>۲۸</t>
         </is>
       </c>
-      <c r="D12" s="10" t="inlineStr">
+      <c r="D12" s="9" t="inlineStr">
         <is>
           <t>17</t>
         </is>
@@ -1108,7 +1088,7 @@
           <t>۲۹</t>
         </is>
       </c>
-      <c r="F12" s="10" t="inlineStr">
+      <c r="F12" s="9" t="inlineStr">
         <is>
           <t>18</t>
         </is>
@@ -1118,7 +1098,7 @@
           <t>۳۰</t>
         </is>
       </c>
-      <c r="H12" s="10" t="inlineStr">
+      <c r="H12" s="9" t="inlineStr">
         <is>
           <t>19</t>
         </is>
@@ -1128,7 +1108,7 @@
           <t>۳۱</t>
         </is>
       </c>
-      <c r="J12" s="10" t="inlineStr">
+      <c r="J12" s="9" t="inlineStr">
         <is>
           <t>20</t>
         </is>
@@ -1474,7 +1454,7 @@
           <t>۱</t>
         </is>
       </c>
-      <c r="L4" s="10" t="inlineStr">
+      <c r="L4" s="9" t="inlineStr">
         <is>
           <t>22</t>
         </is>
@@ -1484,7 +1464,7 @@
           <t>۲</t>
         </is>
       </c>
-      <c r="N4" s="10" t="inlineStr">
+      <c r="N4" s="9" t="inlineStr">
         <is>
           <t>23</t>
         </is>
@@ -1522,7 +1502,7 @@
           <t>۳</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="9" t="inlineStr">
         <is>
           <t>24</t>
         </is>
@@ -1532,7 +1512,7 @@
           <t>۴</t>
         </is>
       </c>
-      <c r="D6" s="10" t="inlineStr">
+      <c r="D6" s="9" t="inlineStr">
         <is>
           <t>25</t>
         </is>
@@ -1542,7 +1522,7 @@
           <t>۵</t>
         </is>
       </c>
-      <c r="F6" s="10" t="inlineStr">
+      <c r="F6" s="9" t="inlineStr">
         <is>
           <t>26</t>
         </is>
@@ -1552,7 +1532,7 @@
           <t>۶</t>
         </is>
       </c>
-      <c r="H6" s="10" t="inlineStr">
+      <c r="H6" s="9" t="inlineStr">
         <is>
           <t>27</t>
         </is>
@@ -1562,7 +1542,7 @@
           <t>۷</t>
         </is>
       </c>
-      <c r="J6" s="10" t="inlineStr">
+      <c r="J6" s="9" t="inlineStr">
         <is>
           <t>28</t>
         </is>
@@ -1572,7 +1552,7 @@
           <t>۸</t>
         </is>
       </c>
-      <c r="L6" s="10" t="inlineStr">
+      <c r="L6" s="9" t="inlineStr">
         <is>
           <t>29</t>
         </is>
@@ -1582,7 +1562,7 @@
           <t>۹</t>
         </is>
       </c>
-      <c r="N6" s="10" t="inlineStr">
+      <c r="N6" s="9" t="inlineStr">
         <is>
           <t>30</t>
         </is>
@@ -1597,7 +1577,7 @@
         </is>
       </c>
       <c r="C7" s="8" t="n"/>
-      <c r="D7" s="12" t="inlineStr">
+      <c r="D7" s="10" t="inlineStr">
         <is>
           <t>١ جمادي الثاني</t>
         </is>
@@ -1640,7 +1620,7 @@
           <t>۱۰</t>
         </is>
       </c>
-      <c r="B8" s="10" t="inlineStr">
+      <c r="B8" s="9" t="inlineStr">
         <is>
           <t>31</t>
         </is>
@@ -1650,7 +1630,7 @@
           <t>۱۱</t>
         </is>
       </c>
-      <c r="D8" s="11" t="inlineStr">
+      <c r="D8" s="10" t="inlineStr">
         <is>
           <t>1 January</t>
         </is>
@@ -1660,7 +1640,7 @@
           <t>۱۲</t>
         </is>
       </c>
-      <c r="F8" s="10" t="inlineStr">
+      <c r="F8" s="9" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -1670,7 +1650,7 @@
           <t>۱۳</t>
         </is>
       </c>
-      <c r="H8" s="10" t="inlineStr">
+      <c r="H8" s="9" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -1680,7 +1660,7 @@
           <t>۱۴</t>
         </is>
       </c>
-      <c r="J8" s="10" t="inlineStr">
+      <c r="J8" s="9" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -1690,7 +1670,7 @@
           <t>۱۵</t>
         </is>
       </c>
-      <c r="L8" s="10" t="inlineStr">
+      <c r="L8" s="9" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -1700,7 +1680,7 @@
           <t>۱۶</t>
         </is>
       </c>
-      <c r="N8" s="10" t="inlineStr">
+      <c r="N8" s="9" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -1758,7 +1738,7 @@
           <t>۱۷</t>
         </is>
       </c>
-      <c r="B10" s="10" t="inlineStr">
+      <c r="B10" s="9" t="inlineStr">
         <is>
           <t>7</t>
         </is>
@@ -1768,7 +1748,7 @@
           <t>۱۸</t>
         </is>
       </c>
-      <c r="D10" s="10" t="inlineStr">
+      <c r="D10" s="9" t="inlineStr">
         <is>
           <t>8</t>
         </is>
@@ -1778,7 +1758,7 @@
           <t>۱۹</t>
         </is>
       </c>
-      <c r="F10" s="10" t="inlineStr">
+      <c r="F10" s="9" t="inlineStr">
         <is>
           <t>9</t>
         </is>
@@ -1788,7 +1768,7 @@
           <t>۲۰</t>
         </is>
       </c>
-      <c r="H10" s="10" t="inlineStr">
+      <c r="H10" s="9" t="inlineStr">
         <is>
           <t>10</t>
         </is>
@@ -1798,7 +1778,7 @@
           <t>۲۱</t>
         </is>
       </c>
-      <c r="J10" s="10" t="inlineStr">
+      <c r="J10" s="9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
@@ -1808,7 +1788,7 @@
           <t>۲۲</t>
         </is>
       </c>
-      <c r="L10" s="10" t="inlineStr">
+      <c r="L10" s="9" t="inlineStr">
         <is>
           <t>12</t>
         </is>
@@ -1818,7 +1798,7 @@
           <t>۲۳</t>
         </is>
       </c>
-      <c r="N10" s="10" t="inlineStr">
+      <c r="N10" s="9" t="inlineStr">
         <is>
           <t>13</t>
         </is>
@@ -1876,7 +1856,7 @@
           <t>۲۴</t>
         </is>
       </c>
-      <c r="B12" s="10" t="inlineStr">
+      <c r="B12" s="9" t="inlineStr">
         <is>
           <t>14</t>
         </is>
@@ -1886,7 +1866,7 @@
           <t>۲۵</t>
         </is>
       </c>
-      <c r="D12" s="10" t="inlineStr">
+      <c r="D12" s="9" t="inlineStr">
         <is>
           <t>15</t>
         </is>
@@ -1896,7 +1876,7 @@
           <t>۲۶</t>
         </is>
       </c>
-      <c r="F12" s="10" t="inlineStr">
+      <c r="F12" s="9" t="inlineStr">
         <is>
           <t>16</t>
         </is>
@@ -1906,7 +1886,7 @@
           <t>۲۷</t>
         </is>
       </c>
-      <c r="H12" s="10" t="inlineStr">
+      <c r="H12" s="9" t="inlineStr">
         <is>
           <t>17</t>
         </is>
@@ -1916,7 +1896,7 @@
           <t>۲۸</t>
         </is>
       </c>
-      <c r="J12" s="10" t="inlineStr">
+      <c r="J12" s="9" t="inlineStr">
         <is>
           <t>18</t>
         </is>
@@ -1926,7 +1906,7 @@
           <t>۲۹</t>
         </is>
       </c>
-      <c r="L12" s="10" t="inlineStr">
+      <c r="L12" s="9" t="inlineStr">
         <is>
           <t>19</t>
         </is>
@@ -1936,7 +1916,7 @@
           <t>۳۰</t>
         </is>
       </c>
-      <c r="N12" s="10" t="inlineStr">
+      <c r="N12" s="9" t="inlineStr">
         <is>
           <t>20</t>
         </is>
@@ -2275,7 +2255,7 @@
           <t>۱</t>
         </is>
       </c>
-      <c r="B4" s="10" t="inlineStr">
+      <c r="B4" s="9" t="inlineStr">
         <is>
           <t>21</t>
         </is>
@@ -2285,7 +2265,7 @@
           <t>۲</t>
         </is>
       </c>
-      <c r="D4" s="10" t="inlineStr">
+      <c r="D4" s="9" t="inlineStr">
         <is>
           <t>22</t>
         </is>
@@ -2295,7 +2275,7 @@
           <t>۳</t>
         </is>
       </c>
-      <c r="F4" s="10" t="inlineStr">
+      <c r="F4" s="9" t="inlineStr">
         <is>
           <t>23</t>
         </is>
@@ -2305,7 +2285,7 @@
           <t>۴</t>
         </is>
       </c>
-      <c r="H4" s="10" t="inlineStr">
+      <c r="H4" s="9" t="inlineStr">
         <is>
           <t>24</t>
         </is>
@@ -2315,7 +2295,7 @@
           <t>۵</t>
         </is>
       </c>
-      <c r="J4" s="10" t="inlineStr">
+      <c r="J4" s="9" t="inlineStr">
         <is>
           <t>25</t>
         </is>
@@ -2325,7 +2305,7 @@
           <t>۶</t>
         </is>
       </c>
-      <c r="L4" s="10" t="inlineStr">
+      <c r="L4" s="9" t="inlineStr">
         <is>
           <t>26</t>
         </is>
@@ -2335,7 +2315,7 @@
           <t>۷</t>
         </is>
       </c>
-      <c r="N4" s="10" t="inlineStr">
+      <c r="N4" s="9" t="inlineStr">
         <is>
           <t>27</t>
         </is>
@@ -2356,7 +2336,7 @@
         </is>
       </c>
       <c r="E5" s="8" t="n"/>
-      <c r="F5" s="12" t="inlineStr">
+      <c r="F5" s="10" t="inlineStr">
         <is>
           <t>١ رجب</t>
         </is>
@@ -2393,7 +2373,7 @@
           <t>۸</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="9" t="inlineStr">
         <is>
           <t>28</t>
         </is>
@@ -2403,7 +2383,7 @@
           <t>۹</t>
         </is>
       </c>
-      <c r="D6" s="10" t="inlineStr">
+      <c r="D6" s="9" t="inlineStr">
         <is>
           <t>29</t>
         </is>
@@ -2413,7 +2393,7 @@
           <t>۱۰</t>
         </is>
       </c>
-      <c r="F6" s="10" t="inlineStr">
+      <c r="F6" s="9" t="inlineStr">
         <is>
           <t>30</t>
         </is>
@@ -2423,7 +2403,7 @@
           <t>۱۱</t>
         </is>
       </c>
-      <c r="H6" s="10" t="inlineStr">
+      <c r="H6" s="9" t="inlineStr">
         <is>
           <t>31</t>
         </is>
@@ -2433,7 +2413,7 @@
           <t>۱۲</t>
         </is>
       </c>
-      <c r="J6" s="11" t="inlineStr">
+      <c r="J6" s="10" t="inlineStr">
         <is>
           <t>1 February</t>
         </is>
@@ -2443,7 +2423,7 @@
           <t>۱۳</t>
         </is>
       </c>
-      <c r="L6" s="10" t="inlineStr">
+      <c r="L6" s="9" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -2453,7 +2433,7 @@
           <t>۱۴</t>
         </is>
       </c>
-      <c r="N6" s="10" t="inlineStr">
+      <c r="N6" s="9" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -2511,7 +2491,7 @@
           <t>۱۵</t>
         </is>
       </c>
-      <c r="B8" s="10" t="inlineStr">
+      <c r="B8" s="9" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -2521,7 +2501,7 @@
           <t>۱۶</t>
         </is>
       </c>
-      <c r="D8" s="10" t="inlineStr">
+      <c r="D8" s="9" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -2531,7 +2511,7 @@
           <t>۱۷</t>
         </is>
       </c>
-      <c r="F8" s="10" t="inlineStr">
+      <c r="F8" s="9" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -2541,7 +2521,7 @@
           <t>۱۸</t>
         </is>
       </c>
-      <c r="H8" s="10" t="inlineStr">
+      <c r="H8" s="9" t="inlineStr">
         <is>
           <t>7</t>
         </is>
@@ -2551,7 +2531,7 @@
           <t>۱۹</t>
         </is>
       </c>
-      <c r="J8" s="10" t="inlineStr">
+      <c r="J8" s="9" t="inlineStr">
         <is>
           <t>8</t>
         </is>
@@ -2561,7 +2541,7 @@
           <t>۲۰</t>
         </is>
       </c>
-      <c r="L8" s="10" t="inlineStr">
+      <c r="L8" s="9" t="inlineStr">
         <is>
           <t>9</t>
         </is>
@@ -2571,7 +2551,7 @@
           <t>۲۱</t>
         </is>
       </c>
-      <c r="N8" s="10" t="inlineStr">
+      <c r="N8" s="9" t="inlineStr">
         <is>
           <t>10</t>
         </is>
@@ -2629,7 +2609,7 @@
           <t>۲۲</t>
         </is>
       </c>
-      <c r="B10" s="10" t="inlineStr">
+      <c r="B10" s="9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
@@ -2639,7 +2619,7 @@
           <t>۲۳</t>
         </is>
       </c>
-      <c r="D10" s="10" t="inlineStr">
+      <c r="D10" s="9" t="inlineStr">
         <is>
           <t>12</t>
         </is>
@@ -2649,7 +2629,7 @@
           <t>۲۴</t>
         </is>
       </c>
-      <c r="F10" s="10" t="inlineStr">
+      <c r="F10" s="9" t="inlineStr">
         <is>
           <t>13</t>
         </is>
@@ -2659,7 +2639,7 @@
           <t>۲۵</t>
         </is>
       </c>
-      <c r="H10" s="10" t="inlineStr">
+      <c r="H10" s="9" t="inlineStr">
         <is>
           <t>14</t>
         </is>
@@ -2669,7 +2649,7 @@
           <t>۲۶</t>
         </is>
       </c>
-      <c r="J10" s="10" t="inlineStr">
+      <c r="J10" s="9" t="inlineStr">
         <is>
           <t>15</t>
         </is>
@@ -2679,7 +2659,7 @@
           <t>۲۷</t>
         </is>
       </c>
-      <c r="L10" s="10" t="inlineStr">
+      <c r="L10" s="9" t="inlineStr">
         <is>
           <t>16</t>
         </is>
@@ -2689,7 +2669,7 @@
           <t>۲۸</t>
         </is>
       </c>
-      <c r="N10" s="10" t="inlineStr">
+      <c r="N10" s="9" t="inlineStr">
         <is>
           <t>17</t>
         </is>
@@ -2747,7 +2727,7 @@
           <t>۲۹</t>
         </is>
       </c>
-      <c r="B12" s="10" t="inlineStr">
+      <c r="B12" s="9" t="inlineStr">
         <is>
           <t>18</t>
         </is>
@@ -2757,7 +2737,7 @@
           <t>۳۰</t>
         </is>
       </c>
-      <c r="D12" s="10" t="inlineStr">
+      <c r="D12" s="9" t="inlineStr">
         <is>
           <t>19</t>
         </is>
@@ -3090,7 +3070,7 @@
           <t>۱</t>
         </is>
       </c>
-      <c r="F4" s="10" t="inlineStr">
+      <c r="F4" s="9" t="inlineStr">
         <is>
           <t>20</t>
         </is>
@@ -3100,7 +3080,7 @@
           <t>۲</t>
         </is>
       </c>
-      <c r="H4" s="10" t="inlineStr">
+      <c r="H4" s="9" t="inlineStr">
         <is>
           <t>21</t>
         </is>
@@ -3110,7 +3090,7 @@
           <t>۳</t>
         </is>
       </c>
-      <c r="J4" s="10" t="inlineStr">
+      <c r="J4" s="9" t="inlineStr">
         <is>
           <t>22</t>
         </is>
@@ -3120,7 +3100,7 @@
           <t>۴</t>
         </is>
       </c>
-      <c r="L4" s="10" t="inlineStr">
+      <c r="L4" s="9" t="inlineStr">
         <is>
           <t>23</t>
         </is>
@@ -3130,7 +3110,7 @@
           <t>۵</t>
         </is>
       </c>
-      <c r="N4" s="10" t="inlineStr">
+      <c r="N4" s="9" t="inlineStr">
         <is>
           <t>24</t>
         </is>
@@ -3155,7 +3135,7 @@
         </is>
       </c>
       <c r="I5" s="8" t="n"/>
-      <c r="J5" s="12" t="inlineStr">
+      <c r="J5" s="10" t="inlineStr">
         <is>
           <t>١ شعبان</t>
         </is>
@@ -3180,7 +3160,7 @@
           <t>۶</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="9" t="inlineStr">
         <is>
           <t>25</t>
         </is>
@@ -3190,7 +3170,7 @@
           <t>۷</t>
         </is>
       </c>
-      <c r="D6" s="10" t="inlineStr">
+      <c r="D6" s="9" t="inlineStr">
         <is>
           <t>26</t>
         </is>
@@ -3200,7 +3180,7 @@
           <t>۸</t>
         </is>
       </c>
-      <c r="F6" s="10" t="inlineStr">
+      <c r="F6" s="9" t="inlineStr">
         <is>
           <t>27</t>
         </is>
@@ -3210,7 +3190,7 @@
           <t>۹</t>
         </is>
       </c>
-      <c r="H6" s="10" t="inlineStr">
+      <c r="H6" s="9" t="inlineStr">
         <is>
           <t>28</t>
         </is>
@@ -3220,7 +3200,7 @@
           <t>۱۰</t>
         </is>
       </c>
-      <c r="J6" s="11" t="inlineStr">
+      <c r="J6" s="10" t="inlineStr">
         <is>
           <t>1 March</t>
         </is>
@@ -3230,7 +3210,7 @@
           <t>۱۱</t>
         </is>
       </c>
-      <c r="L6" s="10" t="inlineStr">
+      <c r="L6" s="9" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -3240,7 +3220,7 @@
           <t>۱۲</t>
         </is>
       </c>
-      <c r="N6" s="10" t="inlineStr">
+      <c r="N6" s="9" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -3298,7 +3278,7 @@
           <t>۱۳</t>
         </is>
       </c>
-      <c r="B8" s="10" t="inlineStr">
+      <c r="B8" s="9" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -3308,7 +3288,7 @@
           <t>۱۴</t>
         </is>
       </c>
-      <c r="D8" s="10" t="inlineStr">
+      <c r="D8" s="9" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -3318,7 +3298,7 @@
           <t>۱۵</t>
         </is>
       </c>
-      <c r="F8" s="10" t="inlineStr">
+      <c r="F8" s="9" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -3328,7 +3308,7 @@
           <t>۱۶</t>
         </is>
       </c>
-      <c r="H8" s="10" t="inlineStr">
+      <c r="H8" s="9" t="inlineStr">
         <is>
           <t>7</t>
         </is>
@@ -3338,7 +3318,7 @@
           <t>۱۷</t>
         </is>
       </c>
-      <c r="J8" s="10" t="inlineStr">
+      <c r="J8" s="9" t="inlineStr">
         <is>
           <t>8</t>
         </is>
@@ -3348,7 +3328,7 @@
           <t>۱۸</t>
         </is>
       </c>
-      <c r="L8" s="10" t="inlineStr">
+      <c r="L8" s="9" t="inlineStr">
         <is>
           <t>9</t>
         </is>
@@ -3358,7 +3338,7 @@
           <t>۱۹</t>
         </is>
       </c>
-      <c r="N8" s="10" t="inlineStr">
+      <c r="N8" s="9" t="inlineStr">
         <is>
           <t>10</t>
         </is>
@@ -3416,7 +3396,7 @@
           <t>۲۰</t>
         </is>
       </c>
-      <c r="B10" s="10" t="inlineStr">
+      <c r="B10" s="9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
@@ -3426,7 +3406,7 @@
           <t>۲۱</t>
         </is>
       </c>
-      <c r="D10" s="10" t="inlineStr">
+      <c r="D10" s="9" t="inlineStr">
         <is>
           <t>12</t>
         </is>
@@ -3436,7 +3416,7 @@
           <t>۲۲</t>
         </is>
       </c>
-      <c r="F10" s="10" t="inlineStr">
+      <c r="F10" s="9" t="inlineStr">
         <is>
           <t>13</t>
         </is>
@@ -3446,7 +3426,7 @@
           <t>۲۳</t>
         </is>
       </c>
-      <c r="H10" s="10" t="inlineStr">
+      <c r="H10" s="9" t="inlineStr">
         <is>
           <t>14</t>
         </is>
@@ -3456,7 +3436,7 @@
           <t>۲۴</t>
         </is>
       </c>
-      <c r="J10" s="10" t="inlineStr">
+      <c r="J10" s="9" t="inlineStr">
         <is>
           <t>15</t>
         </is>
@@ -3466,7 +3446,7 @@
           <t>۲۵</t>
         </is>
       </c>
-      <c r="L10" s="10" t="inlineStr">
+      <c r="L10" s="9" t="inlineStr">
         <is>
           <t>16</t>
         </is>
@@ -3476,7 +3456,7 @@
           <t>۲۶</t>
         </is>
       </c>
-      <c r="N10" s="10" t="inlineStr">
+      <c r="N10" s="9" t="inlineStr">
         <is>
           <t>17</t>
         </is>
@@ -3534,7 +3514,7 @@
           <t>۲۷</t>
         </is>
       </c>
-      <c r="B12" s="10" t="inlineStr">
+      <c r="B12" s="9" t="inlineStr">
         <is>
           <t>18</t>
         </is>
@@ -3544,7 +3524,7 @@
           <t>۲۸</t>
         </is>
       </c>
-      <c r="D12" s="10" t="inlineStr">
+      <c r="D12" s="9" t="inlineStr">
         <is>
           <t>19</t>
         </is>
@@ -3554,7 +3534,7 @@
           <t>۲۹</t>
         </is>
       </c>
-      <c r="F12" s="10" t="inlineStr">
+      <c r="F12" s="9" t="inlineStr">
         <is>
           <t>20</t>
         </is>
@@ -3894,7 +3874,7 @@
           <t>۱</t>
         </is>
       </c>
-      <c r="L4" s="10" t="inlineStr">
+      <c r="L4" s="9" t="inlineStr">
         <is>
           <t>21</t>
         </is>
@@ -3904,7 +3884,7 @@
           <t>۲</t>
         </is>
       </c>
-      <c r="N4" s="10" t="inlineStr">
+      <c r="N4" s="9" t="inlineStr">
         <is>
           <t>22</t>
         </is>
@@ -3942,7 +3922,7 @@
           <t>۳</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="9" t="inlineStr">
         <is>
           <t>23</t>
         </is>
@@ -3952,7 +3932,7 @@
           <t>۴</t>
         </is>
       </c>
-      <c r="D6" s="10" t="inlineStr">
+      <c r="D6" s="9" t="inlineStr">
         <is>
           <t>24</t>
         </is>
@@ -3962,7 +3942,7 @@
           <t>۵</t>
         </is>
       </c>
-      <c r="F6" s="10" t="inlineStr">
+      <c r="F6" s="9" t="inlineStr">
         <is>
           <t>25</t>
         </is>
@@ -3972,7 +3952,7 @@
           <t>۶</t>
         </is>
       </c>
-      <c r="H6" s="10" t="inlineStr">
+      <c r="H6" s="9" t="inlineStr">
         <is>
           <t>26</t>
         </is>
@@ -3982,7 +3962,7 @@
           <t>۷</t>
         </is>
       </c>
-      <c r="J6" s="10" t="inlineStr">
+      <c r="J6" s="9" t="inlineStr">
         <is>
           <t>27</t>
         </is>
@@ -3992,7 +3972,7 @@
           <t>۸</t>
         </is>
       </c>
-      <c r="L6" s="10" t="inlineStr">
+      <c r="L6" s="9" t="inlineStr">
         <is>
           <t>28</t>
         </is>
@@ -4002,7 +3982,7 @@
           <t>۹</t>
         </is>
       </c>
-      <c r="N6" s="10" t="inlineStr">
+      <c r="N6" s="9" t="inlineStr">
         <is>
           <t>29</t>
         </is>
@@ -4060,7 +4040,7 @@
           <t>۱۰</t>
         </is>
       </c>
-      <c r="B8" s="10" t="inlineStr">
+      <c r="B8" s="9" t="inlineStr">
         <is>
           <t>30</t>
         </is>
@@ -4070,7 +4050,7 @@
           <t>۱۱</t>
         </is>
       </c>
-      <c r="D8" s="11" t="inlineStr">
+      <c r="D8" s="10" t="inlineStr">
         <is>
           <t>1 May</t>
         </is>
@@ -4080,7 +4060,7 @@
           <t>۱۲</t>
         </is>
       </c>
-      <c r="F8" s="10" t="inlineStr">
+      <c r="F8" s="9" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -4090,7 +4070,7 @@
           <t>۱۳</t>
         </is>
       </c>
-      <c r="H8" s="10" t="inlineStr">
+      <c r="H8" s="9" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -4100,7 +4080,7 @@
           <t>۱۴</t>
         </is>
       </c>
-      <c r="J8" s="10" t="inlineStr">
+      <c r="J8" s="9" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -4110,7 +4090,7 @@
           <t>۱۵</t>
         </is>
       </c>
-      <c r="L8" s="10" t="inlineStr">
+      <c r="L8" s="9" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -4120,7 +4100,7 @@
           <t>۱۶</t>
         </is>
       </c>
-      <c r="N8" s="10" t="inlineStr">
+      <c r="N8" s="9" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -4147,7 +4127,7 @@
         </is>
       </c>
       <c r="G9" s="8" t="n"/>
-      <c r="H9" s="12" t="inlineStr">
+      <c r="H9" s="10" t="inlineStr">
         <is>
           <t>١ شوال</t>
         </is>
@@ -4178,7 +4158,7 @@
           <t>۱۷</t>
         </is>
       </c>
-      <c r="B10" s="10" t="inlineStr">
+      <c r="B10" s="9" t="inlineStr">
         <is>
           <t>7</t>
         </is>
@@ -4188,7 +4168,7 @@
           <t>۱۸</t>
         </is>
       </c>
-      <c r="D10" s="10" t="inlineStr">
+      <c r="D10" s="9" t="inlineStr">
         <is>
           <t>8</t>
         </is>
@@ -4198,7 +4178,7 @@
           <t>۱۹</t>
         </is>
       </c>
-      <c r="F10" s="10" t="inlineStr">
+      <c r="F10" s="9" t="inlineStr">
         <is>
           <t>9</t>
         </is>
@@ -4208,7 +4188,7 @@
           <t>۲۰</t>
         </is>
       </c>
-      <c r="H10" s="10" t="inlineStr">
+      <c r="H10" s="9" t="inlineStr">
         <is>
           <t>10</t>
         </is>
@@ -4218,7 +4198,7 @@
           <t>۲۱</t>
         </is>
       </c>
-      <c r="J10" s="10" t="inlineStr">
+      <c r="J10" s="9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
@@ -4228,7 +4208,7 @@
           <t>۲۲</t>
         </is>
       </c>
-      <c r="L10" s="10" t="inlineStr">
+      <c r="L10" s="9" t="inlineStr">
         <is>
           <t>12</t>
         </is>
@@ -4238,7 +4218,7 @@
           <t>۲۳</t>
         </is>
       </c>
-      <c r="N10" s="10" t="inlineStr">
+      <c r="N10" s="9" t="inlineStr">
         <is>
           <t>13</t>
         </is>
@@ -4296,7 +4276,7 @@
           <t>۲۴</t>
         </is>
       </c>
-      <c r="B12" s="10" t="inlineStr">
+      <c r="B12" s="9" t="inlineStr">
         <is>
           <t>14</t>
         </is>
@@ -4306,7 +4286,7 @@
           <t>۲۵</t>
         </is>
       </c>
-      <c r="D12" s="10" t="inlineStr">
+      <c r="D12" s="9" t="inlineStr">
         <is>
           <t>15</t>
         </is>
@@ -4316,7 +4296,7 @@
           <t>۲۶</t>
         </is>
       </c>
-      <c r="F12" s="10" t="inlineStr">
+      <c r="F12" s="9" t="inlineStr">
         <is>
           <t>16</t>
         </is>
@@ -4326,7 +4306,7 @@
           <t>۲۷</t>
         </is>
       </c>
-      <c r="H12" s="10" t="inlineStr">
+      <c r="H12" s="9" t="inlineStr">
         <is>
           <t>17</t>
         </is>
@@ -4336,7 +4316,7 @@
           <t>۲۸</t>
         </is>
       </c>
-      <c r="J12" s="10" t="inlineStr">
+      <c r="J12" s="9" t="inlineStr">
         <is>
           <t>18</t>
         </is>
@@ -4346,7 +4326,7 @@
           <t>۲۹</t>
         </is>
       </c>
-      <c r="L12" s="10" t="inlineStr">
+      <c r="L12" s="9" t="inlineStr">
         <is>
           <t>19</t>
         </is>
@@ -4356,7 +4336,7 @@
           <t>۳۰</t>
         </is>
       </c>
-      <c r="N12" s="10" t="inlineStr">
+      <c r="N12" s="9" t="inlineStr">
         <is>
           <t>20</t>
         </is>
@@ -4414,7 +4394,7 @@
           <t>۳۱</t>
         </is>
       </c>
-      <c r="B14" s="10" t="inlineStr">
+      <c r="B14" s="9" t="inlineStr">
         <is>
           <t>21</t>
         </is>
@@ -4710,7 +4690,7 @@
           <t>۱</t>
         </is>
       </c>
-      <c r="D4" s="10" t="inlineStr">
+      <c r="D4" s="9" t="inlineStr">
         <is>
           <t>22</t>
         </is>
@@ -4720,7 +4700,7 @@
           <t>۲</t>
         </is>
       </c>
-      <c r="F4" s="10" t="inlineStr">
+      <c r="F4" s="9" t="inlineStr">
         <is>
           <t>23</t>
         </is>
@@ -4730,7 +4710,7 @@
           <t>۳</t>
         </is>
       </c>
-      <c r="H4" s="10" t="inlineStr">
+      <c r="H4" s="9" t="inlineStr">
         <is>
           <t>24</t>
         </is>
@@ -4740,7 +4720,7 @@
           <t>۴</t>
         </is>
       </c>
-      <c r="J4" s="10" t="inlineStr">
+      <c r="J4" s="9" t="inlineStr">
         <is>
           <t>25</t>
         </is>
@@ -4750,7 +4730,7 @@
           <t>۵</t>
         </is>
       </c>
-      <c r="L4" s="10" t="inlineStr">
+      <c r="L4" s="9" t="inlineStr">
         <is>
           <t>26</t>
         </is>
@@ -4760,7 +4740,7 @@
           <t>۶</t>
         </is>
       </c>
-      <c r="N4" s="10" t="inlineStr">
+      <c r="N4" s="9" t="inlineStr">
         <is>
           <t>27</t>
         </is>
@@ -4814,7 +4794,7 @@
           <t>۷</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="9" t="inlineStr">
         <is>
           <t>28</t>
         </is>
@@ -4824,7 +4804,7 @@
           <t>۸</t>
         </is>
       </c>
-      <c r="D6" s="10" t="inlineStr">
+      <c r="D6" s="9" t="inlineStr">
         <is>
           <t>29</t>
         </is>
@@ -4834,7 +4814,7 @@
           <t>۹</t>
         </is>
       </c>
-      <c r="F6" s="10" t="inlineStr">
+      <c r="F6" s="9" t="inlineStr">
         <is>
           <t>30</t>
         </is>
@@ -4844,7 +4824,7 @@
           <t>۱۰</t>
         </is>
       </c>
-      <c r="H6" s="10" t="inlineStr">
+      <c r="H6" s="9" t="inlineStr">
         <is>
           <t>31</t>
         </is>
@@ -4854,7 +4834,7 @@
           <t>۱۱</t>
         </is>
       </c>
-      <c r="J6" s="11" t="inlineStr">
+      <c r="J6" s="10" t="inlineStr">
         <is>
           <t>1 June</t>
         </is>
@@ -4864,7 +4844,7 @@
           <t>۱۲</t>
         </is>
       </c>
-      <c r="L6" s="10" t="inlineStr">
+      <c r="L6" s="9" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -4874,7 +4854,7 @@
           <t>۱۳</t>
         </is>
       </c>
-      <c r="N6" s="10" t="inlineStr">
+      <c r="N6" s="9" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -4907,7 +4887,7 @@
         </is>
       </c>
       <c r="I7" s="8" t="n"/>
-      <c r="J7" s="12" t="inlineStr">
+      <c r="J7" s="10" t="inlineStr">
         <is>
           <t>١ ذوالقعده</t>
         </is>
@@ -4932,7 +4912,7 @@
           <t>۱۴</t>
         </is>
       </c>
-      <c r="B8" s="10" t="inlineStr">
+      <c r="B8" s="9" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -4942,7 +4922,7 @@
           <t>۱۵</t>
         </is>
       </c>
-      <c r="D8" s="10" t="inlineStr">
+      <c r="D8" s="9" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -4952,7 +4932,7 @@
           <t>۱۶</t>
         </is>
       </c>
-      <c r="F8" s="10" t="inlineStr">
+      <c r="F8" s="9" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -4962,7 +4942,7 @@
           <t>۱۷</t>
         </is>
       </c>
-      <c r="H8" s="10" t="inlineStr">
+      <c r="H8" s="9" t="inlineStr">
         <is>
           <t>7</t>
         </is>
@@ -4972,7 +4952,7 @@
           <t>۱۸</t>
         </is>
       </c>
-      <c r="J8" s="10" t="inlineStr">
+      <c r="J8" s="9" t="inlineStr">
         <is>
           <t>8</t>
         </is>
@@ -4982,7 +4962,7 @@
           <t>۱۹</t>
         </is>
       </c>
-      <c r="L8" s="10" t="inlineStr">
+      <c r="L8" s="9" t="inlineStr">
         <is>
           <t>9</t>
         </is>
@@ -4992,7 +4972,7 @@
           <t>۲۰</t>
         </is>
       </c>
-      <c r="N8" s="10" t="inlineStr">
+      <c r="N8" s="9" t="inlineStr">
         <is>
           <t>10</t>
         </is>
@@ -5050,7 +5030,7 @@
           <t>۲۱</t>
         </is>
       </c>
-      <c r="B10" s="10" t="inlineStr">
+      <c r="B10" s="9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
@@ -5060,7 +5040,7 @@
           <t>۲۲</t>
         </is>
       </c>
-      <c r="D10" s="10" t="inlineStr">
+      <c r="D10" s="9" t="inlineStr">
         <is>
           <t>12</t>
         </is>
@@ -5070,7 +5050,7 @@
           <t>۲۳</t>
         </is>
       </c>
-      <c r="F10" s="10" t="inlineStr">
+      <c r="F10" s="9" t="inlineStr">
         <is>
           <t>13</t>
         </is>
@@ -5080,7 +5060,7 @@
           <t>۲۴</t>
         </is>
       </c>
-      <c r="H10" s="10" t="inlineStr">
+      <c r="H10" s="9" t="inlineStr">
         <is>
           <t>14</t>
         </is>
@@ -5090,7 +5070,7 @@
           <t>۲۵</t>
         </is>
       </c>
-      <c r="J10" s="10" t="inlineStr">
+      <c r="J10" s="9" t="inlineStr">
         <is>
           <t>15</t>
         </is>
@@ -5100,7 +5080,7 @@
           <t>۲۶</t>
         </is>
       </c>
-      <c r="L10" s="10" t="inlineStr">
+      <c r="L10" s="9" t="inlineStr">
         <is>
           <t>16</t>
         </is>
@@ -5110,7 +5090,7 @@
           <t>۲۷</t>
         </is>
       </c>
-      <c r="N10" s="10" t="inlineStr">
+      <c r="N10" s="9" t="inlineStr">
         <is>
           <t>17</t>
         </is>
@@ -5168,7 +5148,7 @@
           <t>۲۸</t>
         </is>
       </c>
-      <c r="B12" s="10" t="inlineStr">
+      <c r="B12" s="9" t="inlineStr">
         <is>
           <t>18</t>
         </is>
@@ -5178,7 +5158,7 @@
           <t>۲۹</t>
         </is>
       </c>
-      <c r="D12" s="10" t="inlineStr">
+      <c r="D12" s="9" t="inlineStr">
         <is>
           <t>19</t>
         </is>
@@ -5188,7 +5168,7 @@
           <t>۳۰</t>
         </is>
       </c>
-      <c r="F12" s="10" t="inlineStr">
+      <c r="F12" s="9" t="inlineStr">
         <is>
           <t>20</t>
         </is>
@@ -5198,7 +5178,7 @@
           <t>۳۱</t>
         </is>
       </c>
-      <c r="H12" s="10" t="inlineStr">
+      <c r="H12" s="9" t="inlineStr">
         <is>
           <t>21</t>
         </is>
@@ -5540,7 +5520,7 @@
           <t>۱</t>
         </is>
       </c>
-      <c r="J4" s="10" t="inlineStr">
+      <c r="J4" s="9" t="inlineStr">
         <is>
           <t>22</t>
         </is>
@@ -5550,7 +5530,7 @@
           <t>۲</t>
         </is>
       </c>
-      <c r="L4" s="10" t="inlineStr">
+      <c r="L4" s="9" t="inlineStr">
         <is>
           <t>23</t>
         </is>
@@ -5560,7 +5540,7 @@
           <t>۳</t>
         </is>
       </c>
-      <c r="N4" s="10" t="inlineStr">
+      <c r="N4" s="9" t="inlineStr">
         <is>
           <t>24</t>
         </is>
@@ -5602,7 +5582,7 @@
           <t>۴</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="9" t="inlineStr">
         <is>
           <t>25</t>
         </is>
@@ -5612,7 +5592,7 @@
           <t>۵</t>
         </is>
       </c>
-      <c r="D6" s="10" t="inlineStr">
+      <c r="D6" s="9" t="inlineStr">
         <is>
           <t>26</t>
         </is>
@@ -5622,7 +5602,7 @@
           <t>۶</t>
         </is>
       </c>
-      <c r="F6" s="10" t="inlineStr">
+      <c r="F6" s="9" t="inlineStr">
         <is>
           <t>27</t>
         </is>
@@ -5632,7 +5612,7 @@
           <t>۷</t>
         </is>
       </c>
-      <c r="H6" s="10" t="inlineStr">
+      <c r="H6" s="9" t="inlineStr">
         <is>
           <t>28</t>
         </is>
@@ -5642,7 +5622,7 @@
           <t>۸</t>
         </is>
       </c>
-      <c r="J6" s="10" t="inlineStr">
+      <c r="J6" s="9" t="inlineStr">
         <is>
           <t>29</t>
         </is>
@@ -5652,7 +5632,7 @@
           <t>۹</t>
         </is>
       </c>
-      <c r="L6" s="10" t="inlineStr">
+      <c r="L6" s="9" t="inlineStr">
         <is>
           <t>30</t>
         </is>
@@ -5662,7 +5642,7 @@
           <t>۱۰</t>
         </is>
       </c>
-      <c r="N6" s="11" t="inlineStr">
+      <c r="N6" s="10" t="inlineStr">
         <is>
           <t>1 July</t>
         </is>
@@ -5707,7 +5687,7 @@
         </is>
       </c>
       <c r="M7" s="8" t="n"/>
-      <c r="N7" s="12" t="inlineStr">
+      <c r="N7" s="10" t="inlineStr">
         <is>
           <t>١ ذوالحجه</t>
         </is>
@@ -5720,7 +5700,7 @@
           <t>۱۱</t>
         </is>
       </c>
-      <c r="B8" s="10" t="inlineStr">
+      <c r="B8" s="9" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -5730,7 +5710,7 @@
           <t>۱۲</t>
         </is>
       </c>
-      <c r="D8" s="10" t="inlineStr">
+      <c r="D8" s="9" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -5740,7 +5720,7 @@
           <t>۱۳</t>
         </is>
       </c>
-      <c r="F8" s="10" t="inlineStr">
+      <c r="F8" s="9" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -5750,7 +5730,7 @@
           <t>۱۴</t>
         </is>
       </c>
-      <c r="H8" s="10" t="inlineStr">
+      <c r="H8" s="9" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -5760,7 +5740,7 @@
           <t>۱۵</t>
         </is>
       </c>
-      <c r="J8" s="10" t="inlineStr">
+      <c r="J8" s="9" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -5770,7 +5750,7 @@
           <t>۱۶</t>
         </is>
       </c>
-      <c r="L8" s="10" t="inlineStr">
+      <c r="L8" s="9" t="inlineStr">
         <is>
           <t>7</t>
         </is>
@@ -5780,7 +5760,7 @@
           <t>۱۷</t>
         </is>
       </c>
-      <c r="N8" s="10" t="inlineStr">
+      <c r="N8" s="9" t="inlineStr">
         <is>
           <t>8</t>
         </is>
@@ -5838,7 +5818,7 @@
           <t>۱۸</t>
         </is>
       </c>
-      <c r="B10" s="10" t="inlineStr">
+      <c r="B10" s="9" t="inlineStr">
         <is>
           <t>9</t>
         </is>
@@ -5848,7 +5828,7 @@
           <t>۱۹</t>
         </is>
       </c>
-      <c r="D10" s="10" t="inlineStr">
+      <c r="D10" s="9" t="inlineStr">
         <is>
           <t>10</t>
         </is>
@@ -5858,7 +5838,7 @@
           <t>۲۰</t>
         </is>
       </c>
-      <c r="F10" s="10" t="inlineStr">
+      <c r="F10" s="9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
@@ -5868,7 +5848,7 @@
           <t>۲۱</t>
         </is>
       </c>
-      <c r="H10" s="10" t="inlineStr">
+      <c r="H10" s="9" t="inlineStr">
         <is>
           <t>12</t>
         </is>
@@ -5878,7 +5858,7 @@
           <t>۲۲</t>
         </is>
       </c>
-      <c r="J10" s="10" t="inlineStr">
+      <c r="J10" s="9" t="inlineStr">
         <is>
           <t>13</t>
         </is>
@@ -5888,7 +5868,7 @@
           <t>۲۳</t>
         </is>
       </c>
-      <c r="L10" s="10" t="inlineStr">
+      <c r="L10" s="9" t="inlineStr">
         <is>
           <t>14</t>
         </is>
@@ -5898,7 +5878,7 @@
           <t>۲۴</t>
         </is>
       </c>
-      <c r="N10" s="10" t="inlineStr">
+      <c r="N10" s="9" t="inlineStr">
         <is>
           <t>15</t>
         </is>
@@ -5956,7 +5936,7 @@
           <t>۲۵</t>
         </is>
       </c>
-      <c r="B12" s="10" t="inlineStr">
+      <c r="B12" s="9" t="inlineStr">
         <is>
           <t>16</t>
         </is>
@@ -5966,7 +5946,7 @@
           <t>۲۶</t>
         </is>
       </c>
-      <c r="D12" s="10" t="inlineStr">
+      <c r="D12" s="9" t="inlineStr">
         <is>
           <t>17</t>
         </is>
@@ -5976,7 +5956,7 @@
           <t>۲۷</t>
         </is>
       </c>
-      <c r="F12" s="10" t="inlineStr">
+      <c r="F12" s="9" t="inlineStr">
         <is>
           <t>18</t>
         </is>
@@ -5986,7 +5966,7 @@
           <t>۲۸</t>
         </is>
       </c>
-      <c r="H12" s="10" t="inlineStr">
+      <c r="H12" s="9" t="inlineStr">
         <is>
           <t>19</t>
         </is>
@@ -5996,7 +5976,7 @@
           <t>۲۹</t>
         </is>
       </c>
-      <c r="J12" s="10" t="inlineStr">
+      <c r="J12" s="9" t="inlineStr">
         <is>
           <t>20</t>
         </is>
@@ -6006,7 +5986,7 @@
           <t>۳۰</t>
         </is>
       </c>
-      <c r="L12" s="10" t="inlineStr">
+      <c r="L12" s="9" t="inlineStr">
         <is>
           <t>21</t>
         </is>
@@ -6016,7 +5996,7 @@
           <t>۳۱</t>
         </is>
       </c>
-      <c r="N12" s="10" t="inlineStr">
+      <c r="N12" s="9" t="inlineStr">
         <is>
           <t>22</t>
         </is>
@@ -6356,7 +6336,7 @@
           <t>۱</t>
         </is>
       </c>
-      <c r="B4" s="10" t="inlineStr">
+      <c r="B4" s="9" t="inlineStr">
         <is>
           <t>23</t>
         </is>
@@ -6366,7 +6346,7 @@
           <t>۲</t>
         </is>
       </c>
-      <c r="D4" s="10" t="inlineStr">
+      <c r="D4" s="9" t="inlineStr">
         <is>
           <t>24</t>
         </is>
@@ -6376,7 +6356,7 @@
           <t>۳</t>
         </is>
       </c>
-      <c r="F4" s="10" t="inlineStr">
+      <c r="F4" s="9" t="inlineStr">
         <is>
           <t>25</t>
         </is>
@@ -6386,7 +6366,7 @@
           <t>۴</t>
         </is>
       </c>
-      <c r="H4" s="10" t="inlineStr">
+      <c r="H4" s="9" t="inlineStr">
         <is>
           <t>26</t>
         </is>
@@ -6396,7 +6376,7 @@
           <t>۵</t>
         </is>
       </c>
-      <c r="J4" s="10" t="inlineStr">
+      <c r="J4" s="9" t="inlineStr">
         <is>
           <t>27</t>
         </is>
@@ -6406,7 +6386,7 @@
           <t>۶</t>
         </is>
       </c>
-      <c r="L4" s="10" t="inlineStr">
+      <c r="L4" s="9" t="inlineStr">
         <is>
           <t>28</t>
         </is>
@@ -6416,7 +6396,7 @@
           <t>۷</t>
         </is>
       </c>
-      <c r="N4" s="10" t="inlineStr">
+      <c r="N4" s="9" t="inlineStr">
         <is>
           <t>29</t>
         </is>
@@ -6474,7 +6454,7 @@
           <t>۸</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="9" t="inlineStr">
         <is>
           <t>30</t>
         </is>
@@ -6484,7 +6464,7 @@
           <t>۹</t>
         </is>
       </c>
-      <c r="D6" s="10" t="inlineStr">
+      <c r="D6" s="9" t="inlineStr">
         <is>
           <t>31</t>
         </is>
@@ -6494,7 +6474,7 @@
           <t>۱۰</t>
         </is>
       </c>
-      <c r="F6" s="11" t="inlineStr">
+      <c r="F6" s="10" t="inlineStr">
         <is>
           <t>1 August</t>
         </is>
@@ -6504,7 +6484,7 @@
           <t>۱۱</t>
         </is>
       </c>
-      <c r="H6" s="10" t="inlineStr">
+      <c r="H6" s="9" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -6514,7 +6494,7 @@
           <t>۱۲</t>
         </is>
       </c>
-      <c r="J6" s="10" t="inlineStr">
+      <c r="J6" s="9" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -6524,7 +6504,7 @@
           <t>۱۳</t>
         </is>
       </c>
-      <c r="L6" s="10" t="inlineStr">
+      <c r="L6" s="9" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -6534,7 +6514,7 @@
           <t>۱۴</t>
         </is>
       </c>
-      <c r="N6" s="10" t="inlineStr">
+      <c r="N6" s="9" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -6543,7 +6523,7 @@
     </row>
     <row r="7" ht="30" customHeight="1">
       <c r="A7" s="8" t="n"/>
-      <c r="B7" s="12" t="inlineStr">
+      <c r="B7" s="10" t="inlineStr">
         <is>
           <t>١ محرم</t>
         </is>
@@ -6592,7 +6572,7 @@
           <t>۱۵</t>
         </is>
       </c>
-      <c r="B8" s="10" t="inlineStr">
+      <c r="B8" s="9" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -6602,7 +6582,7 @@
           <t>۱۶</t>
         </is>
       </c>
-      <c r="D8" s="10" t="inlineStr">
+      <c r="D8" s="9" t="inlineStr">
         <is>
           <t>7</t>
         </is>
@@ -6612,7 +6592,7 @@
           <t>۱۷</t>
         </is>
       </c>
-      <c r="F8" s="10" t="inlineStr">
+      <c r="F8" s="9" t="inlineStr">
         <is>
           <t>8</t>
         </is>
@@ -6622,7 +6602,7 @@
           <t>۱۸</t>
         </is>
       </c>
-      <c r="H8" s="10" t="inlineStr">
+      <c r="H8" s="9" t="inlineStr">
         <is>
           <t>9</t>
         </is>
@@ -6632,7 +6612,7 @@
           <t>۱۹</t>
         </is>
       </c>
-      <c r="J8" s="10" t="inlineStr">
+      <c r="J8" s="9" t="inlineStr">
         <is>
           <t>10</t>
         </is>
@@ -6642,7 +6622,7 @@
           <t>۲۰</t>
         </is>
       </c>
-      <c r="L8" s="10" t="inlineStr">
+      <c r="L8" s="9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
@@ -6652,7 +6632,7 @@
           <t>۲۱</t>
         </is>
       </c>
-      <c r="N8" s="10" t="inlineStr">
+      <c r="N8" s="9" t="inlineStr">
         <is>
           <t>12</t>
         </is>
@@ -6710,7 +6690,7 @@
           <t>۲۲</t>
         </is>
       </c>
-      <c r="B10" s="10" t="inlineStr">
+      <c r="B10" s="9" t="inlineStr">
         <is>
           <t>13</t>
         </is>
@@ -6720,7 +6700,7 @@
           <t>۲۳</t>
         </is>
       </c>
-      <c r="D10" s="10" t="inlineStr">
+      <c r="D10" s="9" t="inlineStr">
         <is>
           <t>14</t>
         </is>
@@ -6730,7 +6710,7 @@
           <t>۲۴</t>
         </is>
       </c>
-      <c r="F10" s="10" t="inlineStr">
+      <c r="F10" s="9" t="inlineStr">
         <is>
           <t>15</t>
         </is>
@@ -6740,7 +6720,7 @@
           <t>۲۵</t>
         </is>
       </c>
-      <c r="H10" s="10" t="inlineStr">
+      <c r="H10" s="9" t="inlineStr">
         <is>
           <t>16</t>
         </is>
@@ -6750,7 +6730,7 @@
           <t>۲۶</t>
         </is>
       </c>
-      <c r="J10" s="10" t="inlineStr">
+      <c r="J10" s="9" t="inlineStr">
         <is>
           <t>17</t>
         </is>
@@ -6760,7 +6740,7 @@
           <t>۲۷</t>
         </is>
       </c>
-      <c r="L10" s="10" t="inlineStr">
+      <c r="L10" s="9" t="inlineStr">
         <is>
           <t>18</t>
         </is>
@@ -6770,7 +6750,7 @@
           <t>۲۸</t>
         </is>
       </c>
-      <c r="N10" s="10" t="inlineStr">
+      <c r="N10" s="9" t="inlineStr">
         <is>
           <t>19</t>
         </is>
@@ -6828,7 +6808,7 @@
           <t>۲۹</t>
         </is>
       </c>
-      <c r="B12" s="10" t="inlineStr">
+      <c r="B12" s="9" t="inlineStr">
         <is>
           <t>20</t>
         </is>
@@ -6838,7 +6818,7 @@
           <t>۳۰</t>
         </is>
       </c>
-      <c r="D12" s="10" t="inlineStr">
+      <c r="D12" s="9" t="inlineStr">
         <is>
           <t>21</t>
         </is>
@@ -6848,7 +6828,7 @@
           <t>۳۱</t>
         </is>
       </c>
-      <c r="F12" s="10" t="inlineStr">
+      <c r="F12" s="9" t="inlineStr">
         <is>
           <t>22</t>
         </is>
@@ -7186,7 +7166,7 @@
           <t>۱</t>
         </is>
       </c>
-      <c r="H4" s="10" t="inlineStr">
+      <c r="H4" s="9" t="inlineStr">
         <is>
           <t>23</t>
         </is>
@@ -7196,7 +7176,7 @@
           <t>۲</t>
         </is>
       </c>
-      <c r="J4" s="10" t="inlineStr">
+      <c r="J4" s="9" t="inlineStr">
         <is>
           <t>24</t>
         </is>
@@ -7206,7 +7186,7 @@
           <t>۳</t>
         </is>
       </c>
-      <c r="L4" s="10" t="inlineStr">
+      <c r="L4" s="9" t="inlineStr">
         <is>
           <t>25</t>
         </is>
@@ -7216,7 +7196,7 @@
           <t>۴</t>
         </is>
       </c>
-      <c r="N4" s="10" t="inlineStr">
+      <c r="N4" s="9" t="inlineStr">
         <is>
           <t>26</t>
         </is>
@@ -7262,7 +7242,7 @@
           <t>۵</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="9" t="inlineStr">
         <is>
           <t>27</t>
         </is>
@@ -7272,7 +7252,7 @@
           <t>۶</t>
         </is>
       </c>
-      <c r="D6" s="10" t="inlineStr">
+      <c r="D6" s="9" t="inlineStr">
         <is>
           <t>28</t>
         </is>
@@ -7282,7 +7262,7 @@
           <t>۷</t>
         </is>
       </c>
-      <c r="F6" s="10" t="inlineStr">
+      <c r="F6" s="9" t="inlineStr">
         <is>
           <t>29</t>
         </is>
@@ -7292,7 +7272,7 @@
           <t>۸</t>
         </is>
       </c>
-      <c r="H6" s="10" t="inlineStr">
+      <c r="H6" s="9" t="inlineStr">
         <is>
           <t>30</t>
         </is>
@@ -7302,7 +7282,7 @@
           <t>۹</t>
         </is>
       </c>
-      <c r="J6" s="10" t="inlineStr">
+      <c r="J6" s="9" t="inlineStr">
         <is>
           <t>31</t>
         </is>
@@ -7312,7 +7292,7 @@
           <t>۱۰</t>
         </is>
       </c>
-      <c r="L6" s="11" t="inlineStr">
+      <c r="L6" s="10" t="inlineStr">
         <is>
           <t>1 September</t>
         </is>
@@ -7322,7 +7302,7 @@
           <t>۱۱</t>
         </is>
       </c>
-      <c r="N6" s="10" t="inlineStr">
+      <c r="N6" s="9" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -7343,7 +7323,7 @@
         </is>
       </c>
       <c r="E7" s="8" t="n"/>
-      <c r="F7" s="12" t="inlineStr">
+      <c r="F7" s="10" t="inlineStr">
         <is>
           <t>١ صفر</t>
         </is>
@@ -7380,7 +7360,7 @@
           <t>۱۲</t>
         </is>
       </c>
-      <c r="B8" s="10" t="inlineStr">
+      <c r="B8" s="9" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -7390,7 +7370,7 @@
           <t>۱۳</t>
         </is>
       </c>
-      <c r="D8" s="10" t="inlineStr">
+      <c r="D8" s="9" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -7400,7 +7380,7 @@
           <t>۱۴</t>
         </is>
       </c>
-      <c r="F8" s="10" t="inlineStr">
+      <c r="F8" s="9" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -7410,7 +7390,7 @@
           <t>۱۵</t>
         </is>
       </c>
-      <c r="H8" s="10" t="inlineStr">
+      <c r="H8" s="9" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -7420,7 +7400,7 @@
           <t>۱۶</t>
         </is>
       </c>
-      <c r="J8" s="10" t="inlineStr">
+      <c r="J8" s="9" t="inlineStr">
         <is>
           <t>7</t>
         </is>
@@ -7430,7 +7410,7 @@
           <t>۱۷</t>
         </is>
       </c>
-      <c r="L8" s="10" t="inlineStr">
+      <c r="L8" s="9" t="inlineStr">
         <is>
           <t>8</t>
         </is>
@@ -7440,7 +7420,7 @@
           <t>۱۸</t>
         </is>
       </c>
-      <c r="N8" s="10" t="inlineStr">
+      <c r="N8" s="9" t="inlineStr">
         <is>
           <t>9</t>
         </is>
@@ -7498,7 +7478,7 @@
           <t>۱۹</t>
         </is>
       </c>
-      <c r="B10" s="10" t="inlineStr">
+      <c r="B10" s="9" t="inlineStr">
         <is>
           <t>10</t>
         </is>
@@ -7508,7 +7488,7 @@
           <t>۲۰</t>
         </is>
       </c>
-      <c r="D10" s="10" t="inlineStr">
+      <c r="D10" s="9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
@@ -7518,7 +7498,7 @@
           <t>۲۱</t>
         </is>
       </c>
-      <c r="F10" s="10" t="inlineStr">
+      <c r="F10" s="9" t="inlineStr">
         <is>
           <t>12</t>
         </is>
@@ -7528,7 +7508,7 @@
           <t>۲۲</t>
         </is>
       </c>
-      <c r="H10" s="10" t="inlineStr">
+      <c r="H10" s="9" t="inlineStr">
         <is>
           <t>13</t>
         </is>
@@ -7538,7 +7518,7 @@
           <t>۲۳</t>
         </is>
       </c>
-      <c r="J10" s="10" t="inlineStr">
+      <c r="J10" s="9" t="inlineStr">
         <is>
           <t>14</t>
         </is>
@@ -7548,7 +7528,7 @@
           <t>۲۴</t>
         </is>
       </c>
-      <c r="L10" s="10" t="inlineStr">
+      <c r="L10" s="9" t="inlineStr">
         <is>
           <t>15</t>
         </is>
@@ -7558,7 +7538,7 @@
           <t>۲۵</t>
         </is>
       </c>
-      <c r="N10" s="10" t="inlineStr">
+      <c r="N10" s="9" t="inlineStr">
         <is>
           <t>16</t>
         </is>
@@ -7616,7 +7596,7 @@
           <t>۲۶</t>
         </is>
       </c>
-      <c r="B12" s="10" t="inlineStr">
+      <c r="B12" s="9" t="inlineStr">
         <is>
           <t>17</t>
         </is>
@@ -7626,7 +7606,7 @@
           <t>۲۷</t>
         </is>
       </c>
-      <c r="D12" s="10" t="inlineStr">
+      <c r="D12" s="9" t="inlineStr">
         <is>
           <t>18</t>
         </is>
@@ -7636,7 +7616,7 @@
           <t>۲۸</t>
         </is>
       </c>
-      <c r="F12" s="10" t="inlineStr">
+      <c r="F12" s="9" t="inlineStr">
         <is>
           <t>19</t>
         </is>
@@ -7646,7 +7626,7 @@
           <t>۲۹</t>
         </is>
       </c>
-      <c r="H12" s="10" t="inlineStr">
+      <c r="H12" s="9" t="inlineStr">
         <is>
           <t>20</t>
         </is>
@@ -7656,7 +7636,7 @@
           <t>۳۰</t>
         </is>
       </c>
-      <c r="J12" s="10" t="inlineStr">
+      <c r="J12" s="9" t="inlineStr">
         <is>
           <t>21</t>
         </is>
@@ -7666,7 +7646,7 @@
           <t>۳۱</t>
         </is>
       </c>
-      <c r="L12" s="10" t="inlineStr">
+      <c r="L12" s="9" t="inlineStr">
         <is>
           <t>22</t>
         </is>
@@ -8016,7 +7996,7 @@
           <t>۱</t>
         </is>
       </c>
-      <c r="N4" s="10" t="inlineStr">
+      <c r="N4" s="9" t="inlineStr">
         <is>
           <t>23</t>
         </is>
@@ -8050,7 +8030,7 @@
           <t>۲</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="9" t="inlineStr">
         <is>
           <t>24</t>
         </is>
@@ -8060,7 +8040,7 @@
           <t>۳</t>
         </is>
       </c>
-      <c r="D6" s="10" t="inlineStr">
+      <c r="D6" s="9" t="inlineStr">
         <is>
           <t>25</t>
         </is>
@@ -8070,7 +8050,7 @@
           <t>۴</t>
         </is>
       </c>
-      <c r="F6" s="10" t="inlineStr">
+      <c r="F6" s="9" t="inlineStr">
         <is>
           <t>26</t>
         </is>
@@ -8080,7 +8060,7 @@
           <t>۵</t>
         </is>
       </c>
-      <c r="H6" s="10" t="inlineStr">
+      <c r="H6" s="9" t="inlineStr">
         <is>
           <t>27</t>
         </is>
@@ -8090,7 +8070,7 @@
           <t>۶</t>
         </is>
       </c>
-      <c r="J6" s="10" t="inlineStr">
+      <c r="J6" s="9" t="inlineStr">
         <is>
           <t>28</t>
         </is>
@@ -8100,7 +8080,7 @@
           <t>۷</t>
         </is>
       </c>
-      <c r="L6" s="10" t="inlineStr">
+      <c r="L6" s="9" t="inlineStr">
         <is>
           <t>29</t>
         </is>
@@ -8110,7 +8090,7 @@
           <t>۸</t>
         </is>
       </c>
-      <c r="N6" s="10" t="inlineStr">
+      <c r="N6" s="9" t="inlineStr">
         <is>
           <t>30</t>
         </is>
@@ -8137,7 +8117,7 @@
         </is>
       </c>
       <c r="G7" s="8" t="n"/>
-      <c r="H7" s="12" t="inlineStr">
+      <c r="H7" s="10" t="inlineStr">
         <is>
           <t>١ ربیع الاول</t>
         </is>
@@ -8168,7 +8148,7 @@
           <t>۹</t>
         </is>
       </c>
-      <c r="B8" s="11" t="inlineStr">
+      <c r="B8" s="10" t="inlineStr">
         <is>
           <t>1 October</t>
         </is>
@@ -8178,7 +8158,7 @@
           <t>۱۰</t>
         </is>
       </c>
-      <c r="D8" s="10" t="inlineStr">
+      <c r="D8" s="9" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -8188,7 +8168,7 @@
           <t>۱۱</t>
         </is>
       </c>
-      <c r="F8" s="10" t="inlineStr">
+      <c r="F8" s="9" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -8198,7 +8178,7 @@
           <t>۱۲</t>
         </is>
       </c>
-      <c r="H8" s="10" t="inlineStr">
+      <c r="H8" s="9" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -8208,7 +8188,7 @@
           <t>۱۳</t>
         </is>
       </c>
-      <c r="J8" s="10" t="inlineStr">
+      <c r="J8" s="9" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -8218,7 +8198,7 @@
           <t>۱۴</t>
         </is>
       </c>
-      <c r="L8" s="10" t="inlineStr">
+      <c r="L8" s="9" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -8228,7 +8208,7 @@
           <t>۱۵</t>
         </is>
       </c>
-      <c r="N8" s="10" t="inlineStr">
+      <c r="N8" s="9" t="inlineStr">
         <is>
           <t>7</t>
         </is>
@@ -8286,7 +8266,7 @@
           <t>۱۶</t>
         </is>
       </c>
-      <c r="B10" s="10" t="inlineStr">
+      <c r="B10" s="9" t="inlineStr">
         <is>
           <t>8</t>
         </is>
@@ -8296,7 +8276,7 @@
           <t>۱۷</t>
         </is>
       </c>
-      <c r="D10" s="10" t="inlineStr">
+      <c r="D10" s="9" t="inlineStr">
         <is>
           <t>9</t>
         </is>
@@ -8306,7 +8286,7 @@
           <t>۱۸</t>
         </is>
       </c>
-      <c r="F10" s="10" t="inlineStr">
+      <c r="F10" s="9" t="inlineStr">
         <is>
           <t>10</t>
         </is>
@@ -8316,7 +8296,7 @@
           <t>۱۹</t>
         </is>
       </c>
-      <c r="H10" s="10" t="inlineStr">
+      <c r="H10" s="9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
@@ -8326,7 +8306,7 @@
           <t>۲۰</t>
         </is>
       </c>
-      <c r="J10" s="10" t="inlineStr">
+      <c r="J10" s="9" t="inlineStr">
         <is>
           <t>12</t>
         </is>
@@ -8336,7 +8316,7 @@
           <t>۲۱</t>
         </is>
       </c>
-      <c r="L10" s="10" t="inlineStr">
+      <c r="L10" s="9" t="inlineStr">
         <is>
           <t>13</t>
         </is>
@@ -8346,7 +8326,7 @@
           <t>۲۲</t>
         </is>
       </c>
-      <c r="N10" s="10" t="inlineStr">
+      <c r="N10" s="9" t="inlineStr">
         <is>
           <t>14</t>
         </is>
@@ -8404,7 +8384,7 @@
           <t>۲۳</t>
         </is>
       </c>
-      <c r="B12" s="10" t="inlineStr">
+      <c r="B12" s="9" t="inlineStr">
         <is>
           <t>15</t>
         </is>
@@ -8414,7 +8394,7 @@
           <t>۲۴</t>
         </is>
       </c>
-      <c r="D12" s="10" t="inlineStr">
+      <c r="D12" s="9" t="inlineStr">
         <is>
           <t>16</t>
         </is>
@@ -8424,7 +8404,7 @@
           <t>۲۵</t>
         </is>
       </c>
-      <c r="F12" s="10" t="inlineStr">
+      <c r="F12" s="9" t="inlineStr">
         <is>
           <t>17</t>
         </is>
@@ -8434,7 +8414,7 @@
           <t>۲۶</t>
         </is>
       </c>
-      <c r="H12" s="10" t="inlineStr">
+      <c r="H12" s="9" t="inlineStr">
         <is>
           <t>18</t>
         </is>
@@ -8444,7 +8424,7 @@
           <t>۲۷</t>
         </is>
       </c>
-      <c r="J12" s="10" t="inlineStr">
+      <c r="J12" s="9" t="inlineStr">
         <is>
           <t>19</t>
         </is>
@@ -8454,7 +8434,7 @@
           <t>۲۸</t>
         </is>
       </c>
-      <c r="L12" s="10" t="inlineStr">
+      <c r="L12" s="9" t="inlineStr">
         <is>
           <t>20</t>
         </is>
@@ -8464,7 +8444,7 @@
           <t>۲۹</t>
         </is>
       </c>
-      <c r="N12" s="10" t="inlineStr">
+      <c r="N12" s="9" t="inlineStr">
         <is>
           <t>21</t>
         </is>
@@ -8522,7 +8502,7 @@
           <t>۳۰</t>
         </is>
       </c>
-      <c r="B14" s="10" t="inlineStr">
+      <c r="B14" s="9" t="inlineStr">
         <is>
           <t>22</t>
         </is>
@@ -8817,7 +8797,7 @@
           <t>۱</t>
         </is>
       </c>
-      <c r="D4" s="10" t="inlineStr">
+      <c r="D4" s="9" t="inlineStr">
         <is>
           <t>23</t>
         </is>
@@ -8827,7 +8807,7 @@
           <t>۲</t>
         </is>
       </c>
-      <c r="F4" s="10" t="inlineStr">
+      <c r="F4" s="9" t="inlineStr">
         <is>
           <t>24</t>
         </is>
@@ -8837,7 +8817,7 @@
           <t>۳</t>
         </is>
       </c>
-      <c r="H4" s="10" t="inlineStr">
+      <c r="H4" s="9" t="inlineStr">
         <is>
           <t>25</t>
         </is>
@@ -8847,7 +8827,7 @@
           <t>۴</t>
         </is>
       </c>
-      <c r="J4" s="10" t="inlineStr">
+      <c r="J4" s="9" t="inlineStr">
         <is>
           <t>26</t>
         </is>
@@ -8857,7 +8837,7 @@
           <t>۵</t>
         </is>
       </c>
-      <c r="L4" s="10" t="inlineStr">
+      <c r="L4" s="9" t="inlineStr">
         <is>
           <t>27</t>
         </is>
@@ -8867,7 +8847,7 @@
           <t>۶</t>
         </is>
       </c>
-      <c r="N4" s="10" t="inlineStr">
+      <c r="N4" s="9" t="inlineStr">
         <is>
           <t>28</t>
         </is>
@@ -8902,7 +8882,7 @@
         </is>
       </c>
       <c r="K5" s="8" t="n"/>
-      <c r="L5" s="12" t="inlineStr">
+      <c r="L5" s="10" t="inlineStr">
         <is>
           <t>١ ربیع الثاني</t>
         </is>
@@ -8921,7 +8901,7 @@
           <t>۷</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="9" t="inlineStr">
         <is>
           <t>29</t>
         </is>
@@ -8931,7 +8911,7 @@
           <t>۸</t>
         </is>
       </c>
-      <c r="D6" s="10" t="inlineStr">
+      <c r="D6" s="9" t="inlineStr">
         <is>
           <t>30</t>
         </is>
@@ -8941,7 +8921,7 @@
           <t>۹</t>
         </is>
       </c>
-      <c r="F6" s="10" t="inlineStr">
+      <c r="F6" s="9" t="inlineStr">
         <is>
           <t>31</t>
         </is>
@@ -8951,7 +8931,7 @@
           <t>۱۰</t>
         </is>
       </c>
-      <c r="H6" s="11" t="inlineStr">
+      <c r="H6" s="10" t="inlineStr">
         <is>
           <t>1 November</t>
         </is>
@@ -8961,7 +8941,7 @@
           <t>۱۱</t>
         </is>
       </c>
-      <c r="J6" s="10" t="inlineStr">
+      <c r="J6" s="9" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -8971,7 +8951,7 @@
           <t>۱۲</t>
         </is>
       </c>
-      <c r="L6" s="10" t="inlineStr">
+      <c r="L6" s="9" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -8981,7 +8961,7 @@
           <t>۱۳</t>
         </is>
       </c>
-      <c r="N6" s="10" t="inlineStr">
+      <c r="N6" s="9" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -9039,7 +9019,7 @@
           <t>۱۴</t>
         </is>
       </c>
-      <c r="B8" s="10" t="inlineStr">
+      <c r="B8" s="9" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -9049,7 +9029,7 @@
           <t>۱۵</t>
         </is>
       </c>
-      <c r="D8" s="10" t="inlineStr">
+      <c r="D8" s="9" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -9059,7 +9039,7 @@
           <t>۱۶</t>
         </is>
       </c>
-      <c r="F8" s="10" t="inlineStr">
+      <c r="F8" s="9" t="inlineStr">
         <is>
           <t>7</t>
         </is>
@@ -9069,7 +9049,7 @@
           <t>۱۷</t>
         </is>
       </c>
-      <c r="H8" s="10" t="inlineStr">
+      <c r="H8" s="9" t="inlineStr">
         <is>
           <t>8</t>
         </is>
@@ -9079,7 +9059,7 @@
           <t>۱۸</t>
         </is>
       </c>
-      <c r="J8" s="10" t="inlineStr">
+      <c r="J8" s="9" t="inlineStr">
         <is>
           <t>9</t>
         </is>
@@ -9089,7 +9069,7 @@
           <t>۱۹</t>
         </is>
       </c>
-      <c r="L8" s="10" t="inlineStr">
+      <c r="L8" s="9" t="inlineStr">
         <is>
           <t>10</t>
         </is>
@@ -9099,7 +9079,7 @@
           <t>۲۰</t>
         </is>
       </c>
-      <c r="N8" s="10" t="inlineStr">
+      <c r="N8" s="9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
@@ -9157,7 +9137,7 @@
           <t>۲۱</t>
         </is>
       </c>
-      <c r="B10" s="10" t="inlineStr">
+      <c r="B10" s="9" t="inlineStr">
         <is>
           <t>12</t>
         </is>
@@ -9167,7 +9147,7 @@
           <t>۲۲</t>
         </is>
       </c>
-      <c r="D10" s="10" t="inlineStr">
+      <c r="D10" s="9" t="inlineStr">
         <is>
           <t>13</t>
         </is>
@@ -9177,7 +9157,7 @@
           <t>۲۳</t>
         </is>
       </c>
-      <c r="F10" s="10" t="inlineStr">
+      <c r="F10" s="9" t="inlineStr">
         <is>
           <t>14</t>
         </is>
@@ -9187,7 +9167,7 @@
           <t>۲۴</t>
         </is>
       </c>
-      <c r="H10" s="10" t="inlineStr">
+      <c r="H10" s="9" t="inlineStr">
         <is>
           <t>15</t>
         </is>
@@ -9197,7 +9177,7 @@
           <t>۲۵</t>
         </is>
       </c>
-      <c r="J10" s="10" t="inlineStr">
+      <c r="J10" s="9" t="inlineStr">
         <is>
           <t>16</t>
         </is>
@@ -9207,7 +9187,7 @@
           <t>۲۶</t>
         </is>
       </c>
-      <c r="L10" s="10" t="inlineStr">
+      <c r="L10" s="9" t="inlineStr">
         <is>
           <t>17</t>
         </is>
@@ -9217,7 +9197,7 @@
           <t>۲۷</t>
         </is>
       </c>
-      <c r="N10" s="10" t="inlineStr">
+      <c r="N10" s="9" t="inlineStr">
         <is>
           <t>18</t>
         </is>
@@ -9275,7 +9255,7 @@
           <t>۲۸</t>
         </is>
       </c>
-      <c r="B12" s="10" t="inlineStr">
+      <c r="B12" s="9" t="inlineStr">
         <is>
           <t>19</t>
         </is>
@@ -9285,7 +9265,7 @@
           <t>۲۹</t>
         </is>
       </c>
-      <c r="D12" s="10" t="inlineStr">
+      <c r="D12" s="9" t="inlineStr">
         <is>
           <t>20</t>
         </is>
@@ -9295,7 +9275,7 @@
           <t>۳۰</t>
         </is>
       </c>
-      <c r="F12" s="10" t="inlineStr">
+      <c r="F12" s="9" t="inlineStr">
         <is>
           <t>21</t>
         </is>
@@ -9632,7 +9612,7 @@
           <t>۱</t>
         </is>
       </c>
-      <c r="H4" s="10" t="inlineStr">
+      <c r="H4" s="9" t="inlineStr">
         <is>
           <t>22</t>
         </is>
@@ -9642,7 +9622,7 @@
           <t>۲</t>
         </is>
       </c>
-      <c r="J4" s="10" t="inlineStr">
+      <c r="J4" s="9" t="inlineStr">
         <is>
           <t>23</t>
         </is>
@@ -9652,7 +9632,7 @@
           <t>۳</t>
         </is>
       </c>
-      <c r="L4" s="10" t="inlineStr">
+      <c r="L4" s="9" t="inlineStr">
         <is>
           <t>24</t>
         </is>
@@ -9662,7 +9642,7 @@
           <t>۴</t>
         </is>
       </c>
-      <c r="N4" s="10" t="inlineStr">
+      <c r="N4" s="9" t="inlineStr">
         <is>
           <t>25</t>
         </is>
@@ -9695,7 +9675,7 @@
         </is>
       </c>
       <c r="M5" s="8" t="n"/>
-      <c r="N5" s="12" t="inlineStr">
+      <c r="N5" s="10" t="inlineStr">
         <is>
           <t>١ جمادي الاول</t>
         </is>
@@ -9708,7 +9688,7 @@
           <t>۵</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="9" t="inlineStr">
         <is>
           <t>26</t>
         </is>
@@ -9718,7 +9698,7 @@
           <t>۶</t>
         </is>
       </c>
-      <c r="D6" s="10" t="inlineStr">
+      <c r="D6" s="9" t="inlineStr">
         <is>
           <t>27</t>
         </is>
@@ -9728,7 +9708,7 @@
           <t>۷</t>
         </is>
       </c>
-      <c r="F6" s="10" t="inlineStr">
+      <c r="F6" s="9" t="inlineStr">
         <is>
           <t>28</t>
         </is>
@@ -9738,7 +9718,7 @@
           <t>۸</t>
         </is>
       </c>
-      <c r="H6" s="10" t="inlineStr">
+      <c r="H6" s="9" t="inlineStr">
         <is>
           <t>29</t>
         </is>
@@ -9748,7 +9728,7 @@
           <t>۹</t>
         </is>
       </c>
-      <c r="J6" s="10" t="inlineStr">
+      <c r="J6" s="9" t="inlineStr">
         <is>
           <t>30</t>
         </is>
@@ -9758,7 +9738,7 @@
           <t>۱۰</t>
         </is>
       </c>
-      <c r="L6" s="11" t="inlineStr">
+      <c r="L6" s="10" t="inlineStr">
         <is>
           <t>1 December</t>
         </is>
@@ -9768,7 +9748,7 @@
           <t>۱۱</t>
         </is>
       </c>
-      <c r="N6" s="10" t="inlineStr">
+      <c r="N6" s="9" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -9826,7 +9806,7 @@
           <t>۱۲</t>
         </is>
       </c>
-      <c r="B8" s="10" t="inlineStr">
+      <c r="B8" s="9" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -9836,7 +9816,7 @@
           <t>۱۳</t>
         </is>
       </c>
-      <c r="D8" s="10" t="inlineStr">
+      <c r="D8" s="9" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -9846,7 +9826,7 @@
           <t>۱۴</t>
         </is>
       </c>
-      <c r="F8" s="10" t="inlineStr">
+      <c r="F8" s="9" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -9856,7 +9836,7 @@
           <t>۱۵</t>
         </is>
       </c>
-      <c r="H8" s="10" t="inlineStr">
+      <c r="H8" s="9" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -9866,7 +9846,7 @@
           <t>۱۶</t>
         </is>
       </c>
-      <c r="J8" s="10" t="inlineStr">
+      <c r="J8" s="9" t="inlineStr">
         <is>
           <t>7</t>
         </is>
@@ -9876,7 +9856,7 @@
           <t>۱۷</t>
         </is>
       </c>
-      <c r="L8" s="10" t="inlineStr">
+      <c r="L8" s="9" t="inlineStr">
         <is>
           <t>8</t>
         </is>
@@ -9886,7 +9866,7 @@
           <t>۱۸</t>
         </is>
       </c>
-      <c r="N8" s="10" t="inlineStr">
+      <c r="N8" s="9" t="inlineStr">
         <is>
           <t>9</t>
         </is>
@@ -9944,7 +9924,7 @@
           <t>۱۹</t>
         </is>
       </c>
-      <c r="B10" s="10" t="inlineStr">
+      <c r="B10" s="9" t="inlineStr">
         <is>
           <t>10</t>
         </is>
@@ -9954,7 +9934,7 @@
           <t>۲۰</t>
         </is>
       </c>
-      <c r="D10" s="10" t="inlineStr">
+      <c r="D10" s="9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
@@ -9964,7 +9944,7 @@
           <t>۲۱</t>
         </is>
       </c>
-      <c r="F10" s="10" t="inlineStr">
+      <c r="F10" s="9" t="inlineStr">
         <is>
           <t>12</t>
         </is>
@@ -9974,7 +9954,7 @@
           <t>۲۲</t>
         </is>
       </c>
-      <c r="H10" s="10" t="inlineStr">
+      <c r="H10" s="9" t="inlineStr">
         <is>
           <t>13</t>
         </is>
@@ -9984,7 +9964,7 @@
           <t>۲۳</t>
         </is>
       </c>
-      <c r="J10" s="10" t="inlineStr">
+      <c r="J10" s="9" t="inlineStr">
         <is>
           <t>14</t>
         </is>
@@ -9994,7 +9974,7 @@
           <t>۲۴</t>
         </is>
       </c>
-      <c r="L10" s="10" t="inlineStr">
+      <c r="L10" s="9" t="inlineStr">
         <is>
           <t>15</t>
         </is>
@@ -10004,7 +9984,7 @@
           <t>۲۵</t>
         </is>
       </c>
-      <c r="N10" s="10" t="inlineStr">
+      <c r="N10" s="9" t="inlineStr">
         <is>
           <t>16</t>
         </is>
@@ -10062,7 +10042,7 @@
           <t>۲۶</t>
         </is>
       </c>
-      <c r="B12" s="10" t="inlineStr">
+      <c r="B12" s="9" t="inlineStr">
         <is>
           <t>17</t>
         </is>
@@ -10072,7 +10052,7 @@
           <t>۲۷</t>
         </is>
       </c>
-      <c r="D12" s="10" t="inlineStr">
+      <c r="D12" s="9" t="inlineStr">
         <is>
           <t>18</t>
         </is>
@@ -10082,7 +10062,7 @@
           <t>۲۸</t>
         </is>
       </c>
-      <c r="F12" s="10" t="inlineStr">
+      <c r="F12" s="9" t="inlineStr">
         <is>
           <t>19</t>
         </is>
@@ -10092,7 +10072,7 @@
           <t>۲۹</t>
         </is>
       </c>
-      <c r="H12" s="10" t="inlineStr">
+      <c r="H12" s="9" t="inlineStr">
         <is>
           <t>20</t>
         </is>
@@ -10102,7 +10082,7 @@
           <t>۳۰</t>
         </is>
       </c>
-      <c r="J12" s="10" t="inlineStr">
+      <c r="J12" s="9" t="inlineStr">
         <is>
           <t>21</t>
         </is>

</xml_diff>